<commit_message>
Feat(dashboard): Complete Dashboard Documentation and KPIs
Adds Section 6 ("Dashboard") to the readme.md, documenting the new client-specific analysis area. This commit includes:

Description of the setup, unique customer list, and Data Validation (dropdowns).

Documentation of all four KPI tables and their respective formulas (SUMIF/S and COUNTIF/S) for calculating total billed and outstanding amounts.

Insertion of the final screenshot reference (Screenshot 5) that visually documents the interface and formulas.
</commit_message>
<xml_diff>
--- a/Customer_Invoice_Analysis - filled.xlsx
+++ b/Customer_Invoice_Analysis - filled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\invoice-analysis-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819FF802-C8F2-46EE-841D-10C06F00C86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A8D8A6-B127-4040-99B6-0F4FE14EF85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{56643878-06B9-462D-81B7-435828026F01}"/>
   </bookViews>
@@ -314,7 +314,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -368,14 +368,23 @@
     <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -386,7 +395,7 @@
     <cellStyle name="Normale_Scadenziario crediti" xfId="1" xr:uid="{35419C30-1153-464C-BF4A-8DC9B04ED9AD}"/>
     <cellStyle name="Valuta 7" xfId="3" xr:uid="{C47ED96A-AAD7-4410-AB8F-412DFEB855FF}"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -408,16 +417,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4667,8 +4666,8 @@
   <dimension ref="A1:I201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10823,19 +10822,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A164D69F-5719-4ECE-A976-CD9A45525F6C}">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.08984375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="22.81640625" customWidth="1"/>
-    <col min="4" max="4" width="21.36328125" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" customWidth="1"/>
-    <col min="6" max="6" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="28.90625" customWidth="1"/>
+    <col min="4" max="4" width="28.81640625" customWidth="1"/>
+    <col min="5" max="6" width="6.36328125" customWidth="1"/>
     <col min="7" max="7" width="20.90625" customWidth="1"/>
-    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="8" max="8" width="50.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
@@ -10847,14 +10845,14 @@
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="G2" s="19" t="s">
+      <c r="D2" s="21"/>
+      <c r="G2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="20"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -10881,20 +10879,28 @@
         <v>10</v>
       </c>
       <c r="D4" s="17">
-        <f>COUNTIF(Analysis_Sheet!C:C, C4)</f>
+        <f>COUNTIF(Analysis_Sheet!C:C, Dashboard!C4)</f>
         <v>9</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="19">
         <f>COUNTIFS(Analysis_Sheet!C:C, G4, Analysis_Sheet!H:H, "Overdue") + COUNTIFS(Analysis_Sheet!C:C, G4, Analysis_Sheet!H:H, "Unpaid")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" s="23" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(D4)</f>
+        <v>=CONTA.SE(Analysis_Sheet!C:C; Dashboard!C4)</v>
+      </c>
+      <c r="H5" s="22" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(H4)</f>
+        <v>=CONTA.PIÙ.SE(Analysis_Sheet!C:C; G4; Analysis_Sheet!H:H; "Overdue") + CONTA.PIÙ.SE(Analysis_Sheet!C:C; G4; Analysis_Sheet!H:H; "Unpaid")</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -10916,14 +10922,14 @@
       <c r="A9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="G9" s="19" t="s">
+      <c r="D9" s="21"/>
+      <c r="G9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="20"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
@@ -10950,7 +10956,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="18">
-        <f>SUMIF(Analysis_Sheet!C:C,Dashboard!C11, Analysis_Sheet!D:D )</f>
+        <f>SUMIF(Analysis_Sheet!C:C,C11, Analysis_Sheet!D:D )</f>
         <v>28290.74</v>
       </c>
       <c r="G11" s="16" t="s">
@@ -10961,9 +10967,17 @@
         <v>5050.8999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>15</v>
+      </c>
+      <c r="D12" s="23" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(D11)</f>
+        <v>=SOMMA.SE(Analysis_Sheet!C:C;C11; Analysis_Sheet!D:D )</v>
+      </c>
+      <c r="H12" s="24" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(H11)</f>
+        <v>=SOMMA.PIÙ.SE(Analysis_Sheet!D:D; Analysis_Sheet!C:C; G11; Analysis_Sheet!H:H; "Overdue") + SOMMA.PIÙ.SE(Analysis_Sheet!D:D; Analysis_Sheet!C:C; G11; Analysis_Sheet!H:H; "Unpaid")</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -11550,11 +11564,8 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="G9:H9"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 G11" xr:uid="{DF3C6C81-16D2-4586-94DA-3AE0330AC6DC}">
-      <formula1>$A$2:$A$17</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4 G4" xr:uid="{E36DAA60-4B51-44D5-B5C1-6DA769F7E156}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 G11 C4 G4" xr:uid="{DF3C6C81-16D2-4586-94DA-3AE0330AC6DC}">
       <formula1>$A$2:$A$17</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
FEAT: Complete core analysis, Reporting setup, and README Section 7
Adds essential calculations (Days Overdue, Status) in Analysis_Sheet. Implements the first Pivot Table (Count) and Pie Chart in the Reporting sheet, with final formatting. Updates the README with detailed documentation and two screenshots for the status distribution report.
</commit_message>
<xml_diff>
--- a/Customer_Invoice_Analysis - filled.xlsx
+++ b/Customer_Invoice_Analysis - filled.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\invoice-analysis-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A8D8A6-B127-4040-99B6-0F4FE14EF85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721774B7-958E-4149-A890-92053AAA32D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{56643878-06B9-462D-81B7-435828026F01}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{56643878-06B9-462D-81B7-435828026F01}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice_Master_Data" sheetId="1" r:id="rId1"/>
     <sheet name="Analysis_Sheet" sheetId="2" r:id="rId2"/>
     <sheet name="Dashboard" sheetId="3" r:id="rId3"/>
+    <sheet name="Reporting" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="38">
   <si>
     <t>Sereni</t>
   </si>
@@ -135,6 +139,21 @@
   </si>
   <si>
     <t>Total Amount Billed</t>
+  </si>
+  <si>
+    <t>Overdue</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Unpaid</t>
+  </si>
+  <si>
+    <t>Count of Invoice Number</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -314,7 +333,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -371,21 +390,20 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Colore 3" xfId="5" builtinId="39"/>
@@ -422,6 +440,16 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3333"/>
+      <color rgb="FF72AF2F"/>
+      <color rgb="FF85CA3A"/>
+      <color rgb="FFFF5D5D"/>
+      <color rgb="FFFF8B8B"/>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -431,6 +459,3740 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Customer_Invoice_Analysis - filled.xlsx]Reporting!Tabella pivot1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Invoice</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Status Percentages</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.29305555555555557"/>
+          <c:y val="4.0645960921551476E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="72AF2F"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="-5.6396544181977253E-2"/>
+              <c:y val="-1.1127150772820064E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:spPr>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FF3333"/>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="25400">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d contourW="25400">
+            <a:contourClr>
+              <a:schemeClr val="lt1"/>
+            </a:contourClr>
+          </a:sp3d>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="0.1136334208223972"/>
+              <c:y val="-8.4259259259259256E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:spPr>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="25000"/>
+                  <a:lumOff val="75000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <a:prstGeom prst="wedgeRectCallout">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+              </c15:spPr>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="180"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="40"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reporting!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Totale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d contourW="25400">
+              <a:contourClr>
+                <a:schemeClr val="lt1"/>
+              </a:contourClr>
+            </a:sp3d>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF3333"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7514-443A-A239-FE903773C8F8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="72AF2F"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-7514-443A-A239-FE903773C8F8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-7514-443A-A239-FE903773C8F8}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.6396544181977253E-2"/>
+                  <c:y val="-1.1127150772820064E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-7514-443A-A239-FE903773C8F8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.1136334208223972"/>
+                  <c:y val="-8.4259259259259256E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-7514-443A-A239-FE903773C8F8}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Reporting!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Overdue</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Paid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unpaid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reporting!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7514-443A-A239-FE903773C8F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.74861111111111112"/>
+          <c:y val="0.19146908719743369"/>
+          <c:w val="0.20569210866752913"/>
+          <c:h val="0.30555500182730322"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="262">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E080866D-4932-3BAB-E70C-595520C819A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Admin" refreshedDate="45988.895709027776" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="200" xr:uid="{9D459BF5-FA3A-4137-9408-AD19C132E9EC}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:I201" sheet="Analysis_Sheet"/>
+  </cacheSource>
+  <cacheFields count="9">
+    <cacheField name="Invoice Number" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="200"/>
+    </cacheField>
+    <cacheField name="Issue Date" numFmtId="0">
+      <sharedItems containsDate="1" containsMixedTypes="1" minDate="2024-09-12T00:00:00" maxDate="2026-04-29T00:00:00"/>
+    </cacheField>
+    <cacheField name="Customer" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Amount" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="60" maxValue="23456"/>
+    </cacheField>
+    <cacheField name="Due Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2025-03-01T00:00:00" maxDate="2026-07-29T00:00:00"/>
+    </cacheField>
+    <cacheField name="Payment Date" numFmtId="14">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-03-01T00:00:00" maxDate="2026-07-21T00:00:00"/>
+    </cacheField>
+    <cacheField name="Reference Date" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2025-11-20T00:00:00" maxDate="2025-11-21T00:00:00"/>
+    </cacheField>
+    <cacheField name="Calculated Status" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Paid"/>
+        <s v="Unpaid"/>
+        <s v="Overdue"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Days Overdue" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="230"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="200">
+  <r>
+    <n v="1"/>
+    <d v="2025-05-25T00:00:00"/>
+    <s v="Rossi M."/>
+    <n v="450"/>
+    <d v="2025-08-25T00:00:00"/>
+    <d v="2025-08-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <d v="2025-12-10T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="3562"/>
+    <d v="2026-03-10T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <d v="2025-02-01T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="2700"/>
+    <d v="2025-05-01T00:00:00"/>
+    <d v="2025-05-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <d v="2025-06-15T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="399.36"/>
+    <d v="2025-09-15T00:00:00"/>
+    <d v="2025-10-05T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <d v="2025-08-05T00:00:00"/>
+    <s v="Villani"/>
+    <n v="960"/>
+    <d v="2025-11-05T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <d v="2026-04-20T00:00:00"/>
+    <s v="Bianchi R."/>
+    <n v="7916.67"/>
+    <d v="2026-07-20T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <d v="2025-01-11T00:00:00"/>
+    <s v="Lanza A."/>
+    <n v="3360"/>
+    <d v="2025-04-11T00:00:00"/>
+    <d v="2025-05-11T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <d v="2025-10-03T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="1839.36"/>
+    <d v="2026-01-03T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <d v="2024-12-18T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="477.48"/>
+    <d v="2025-03-18T00:00:00"/>
+    <d v="2025-03-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <d v="2025-11-02T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="750"/>
+    <d v="2026-02-02T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <d v="2025-01-29T00:00:00"/>
+    <s v="Risti"/>
+    <n v="750"/>
+    <d v="2025-04-29T00:00:00"/>
+    <d v="2025-05-05T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <d v="2025-09-14T00:00:00"/>
+    <s v="Rossi F."/>
+    <n v="3284.5"/>
+    <d v="2025-12-14T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <d v="2025-04-08T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="4320"/>
+    <d v="2025-07-08T00:00:00"/>
+    <d v="2025-08-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <d v="2025-10-22T00:00:00"/>
+    <s v="Bianchi A."/>
+    <n v="9600"/>
+    <d v="2026-01-22T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <d v="2026-01-17T00:00:00"/>
+    <s v="Villani"/>
+    <n v="234"/>
+    <d v="2026-04-17T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="16"/>
+    <d v="2025-03-06T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="12000"/>
+    <d v="2025-06-06T00:00:00"/>
+    <d v="2025-06-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <d v="2025-12-09T00:00:00"/>
+    <s v="Risti"/>
+    <n v="123"/>
+    <d v="2026-03-09T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <d v="2025-11-19T00:00:00"/>
+    <s v="Villani"/>
+    <n v="790"/>
+    <d v="2026-02-19T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <d v="2025-01-21T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="580"/>
+    <d v="2025-04-21T00:00:00"/>
+    <d v="2025-04-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <d v="2025-07-04T00:00:00"/>
+    <s v="Lanza C."/>
+    <n v="2112.6"/>
+    <d v="2025-10-04T00:00:00"/>
+    <d v="2025-11-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <d v="2025-12-07T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="1980"/>
+    <d v="2026-03-07T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <d v="2025-09-23T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="534"/>
+    <d v="2025-12-23T00:00:00"/>
+    <d v="2026-01-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <d v="2026-02-13T00:00:00"/>
+    <s v="Risti"/>
+    <n v="8600"/>
+    <d v="2026-05-13T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <d v="2025-04-01T00:00:00"/>
+    <s v="Villani"/>
+    <n v="1600"/>
+    <d v="2025-07-01T00:00:00"/>
+    <d v="2025-07-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <d v="2025-12-17T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="1050"/>
+    <d v="2026-03-17T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <d v="2025-02-28T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="4100"/>
+    <d v="2025-05-28T00:00:00"/>
+    <d v="2025-06-05T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <d v="2025-08-02T00:00:00"/>
+    <s v="Lanza A."/>
+    <n v="20112.62"/>
+    <d v="2025-11-02T00:00:00"/>
+    <d v="2025-11-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <d v="2025-10-11T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="1450"/>
+    <d v="2026-01-11T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <d v="2025-01-04T00:00:00"/>
+    <s v="Marini E."/>
+    <n v="23456"/>
+    <d v="2025-04-04T00:00:00"/>
+    <d v="2025-04-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <d v="2025-03-16T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="400"/>
+    <d v="2025-06-16T00:00:00"/>
+    <d v="2025-06-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <d v="2025-11-27T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="750"/>
+    <d v="2026-02-27T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <d v="2026-01-12T00:00:00"/>
+    <s v="Lanza C."/>
+    <n v="3400"/>
+    <d v="2026-04-12T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <d v="2025-06-05T00:00:00"/>
+    <s v="Villani"/>
+    <n v="1560"/>
+    <d v="2025-09-05T00:00:00"/>
+    <d v="2025-10-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <d v="2024-12-20T00:00:00"/>
+    <s v="Rossi M."/>
+    <n v="2100"/>
+    <d v="2025-03-20T00:00:00"/>
+    <d v="2025-03-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <d v="2025-08-13T00:00:00"/>
+    <s v="Bianchi A."/>
+    <n v="9600"/>
+    <d v="2025-11-13T00:00:00"/>
+    <d v="2025-11-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <d v="2025-05-09T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="4259.9399999999996"/>
+    <d v="2025-08-09T00:00:00"/>
+    <d v="2025-09-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <d v="2025-07-24T00:00:00"/>
+    <s v="Lanza A."/>
+    <n v="230"/>
+    <d v="2025-10-24T00:00:00"/>
+    <d v="2025-11-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <d v="2026-02-03T00:00:00"/>
+    <s v="Villani"/>
+    <n v="3200"/>
+    <d v="2026-05-03T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <d v="2024-12-15T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="6780"/>
+    <d v="2025-03-15T00:00:00"/>
+    <d v="2025-03-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <d v="2025-10-21T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="477.48"/>
+    <d v="2026-01-21T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="41"/>
+    <d v="2025-09-10T00:00:00"/>
+    <s v="Risti"/>
+    <n v="2900"/>
+    <d v="2025-12-10T00:00:00"/>
+    <d v="2025-12-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="42"/>
+    <d v="2025-05-28T00:00:00"/>
+    <s v="Marini G."/>
+    <n v="60"/>
+    <d v="2025-08-28T00:00:00"/>
+    <d v="2025-09-05T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <d v="2025-03-01T00:00:00"/>
+    <s v="Lanza C."/>
+    <n v="3284.5"/>
+    <d v="2025-06-01T00:00:00"/>
+    <d v="2025-06-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <d v="2026-01-07T00:00:00"/>
+    <s v="Villani"/>
+    <n v="750"/>
+    <d v="2026-04-07T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <d v="2026-02-26T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="7356"/>
+    <d v="2026-05-26T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="46"/>
+    <d v="2025-08-19T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="3562"/>
+    <d v="2025-11-19T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="47"/>
+    <d v="2025-12-14T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="12000"/>
+    <d v="2026-03-14T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <d v="2025-07-20T00:00:00"/>
+    <s v="Rossi F."/>
+    <n v="10200"/>
+    <d v="2025-10-20T00:00:00"/>
+    <d v="2025-11-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="49"/>
+    <d v="2026-02-10T00:00:00"/>
+    <s v="Villani"/>
+    <n v="140"/>
+    <d v="2026-05-10T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="50"/>
+    <d v="2025-06-16T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="10900"/>
+    <d v="2025-09-16T00:00:00"/>
+    <d v="2025-09-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="51"/>
+    <d v="2025-04-28T00:00:00"/>
+    <s v="Lanza A."/>
+    <n v="2500"/>
+    <d v="2025-07-28T00:00:00"/>
+    <d v="2026-04-17T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="52"/>
+    <d v="2026-02-10T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="8800"/>
+    <d v="2026-05-10T00:00:00"/>
+    <d v="2026-01-26T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="53"/>
+    <d v="2024-09-12T00:00:00"/>
+    <s v="Marini E."/>
+    <n v="1950"/>
+    <d v="2025-03-12T00:00:00"/>
+    <d v="2026-03-25T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="54"/>
+    <d v="2025-06-04T00:00:00"/>
+    <s v="Rossi M."/>
+    <n v="4789.84"/>
+    <d v="2025-09-04T00:00:00"/>
+    <d v="2025-11-05T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="55"/>
+    <d v="2025-09-17T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="350"/>
+    <d v="2025-12-17T00:00:00"/>
+    <d v="2026-05-02T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="56"/>
+    <d v="2026-04-22T00:00:00"/>
+    <s v="Bianchi R."/>
+    <n v="1700"/>
+    <d v="2026-07-22T00:00:00"/>
+    <d v="2025-06-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="57"/>
+    <d v="2026-01-05T00:00:00"/>
+    <s v="Villani"/>
+    <n v="4600"/>
+    <d v="2026-04-05T00:00:00"/>
+    <d v="2025-08-28T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="58"/>
+    <d v="2025-10-13T00:00:00"/>
+    <s v="Lanza C."/>
+    <n v="550"/>
+    <d v="2026-01-13T00:00:00"/>
+    <d v="2025-12-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="59"/>
+    <s v="29/02/2025"/>
+    <s v="Sereni"/>
+    <n v="10500"/>
+    <d v="2025-05-29T00:00:00"/>
+    <d v="2026-03-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="60"/>
+    <d v="2025-08-08T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="2500"/>
+    <d v="2025-11-08T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <n v="61"/>
+    <d v="2026-01-11T00:00:00"/>
+    <s v="Marini G."/>
+    <n v="1900"/>
+    <d v="2026-04-11T00:00:00"/>
+    <d v="2026-01-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="62"/>
+    <d v="2025-12-20T00:00:00"/>
+    <s v="Risti"/>
+    <n v="8400"/>
+    <d v="2026-03-20T00:00:00"/>
+    <d v="2026-07-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="63"/>
+    <d v="2025-11-07T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="3200"/>
+    <d v="2026-02-07T00:00:00"/>
+    <d v="2026-05-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="64"/>
+    <d v="2025-07-16T00:00:00"/>
+    <s v="Rossi F."/>
+    <n v="4700"/>
+    <d v="2025-10-16T00:00:00"/>
+    <d v="2026-03-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="65"/>
+    <d v="2026-02-02T00:00:00"/>
+    <s v="Villani"/>
+    <n v="1150"/>
+    <d v="2026-05-02T00:00:00"/>
+    <d v="2025-09-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="66"/>
+    <d v="2025-03-14T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="5300"/>
+    <d v="2025-06-14T00:00:00"/>
+    <d v="2025-11-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="67"/>
+    <d v="2025-05-21T00:00:00"/>
+    <s v="Bianchi A."/>
+    <n v="15000"/>
+    <d v="2025-08-21T00:00:00"/>
+    <d v="2026-03-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="68"/>
+    <d v="2025-09-10T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="650"/>
+    <d v="2025-12-10T00:00:00"/>
+    <d v="2026-01-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="69"/>
+    <d v="2025-10-26T00:00:00"/>
+    <s v="Lanza A."/>
+    <n v="2800"/>
+    <d v="2026-01-26T00:00:00"/>
+    <d v="2025-03-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="70"/>
+    <d v="2025-12-03T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="1850"/>
+    <d v="2026-03-03T00:00:00"/>
+    <d v="2025-11-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="71"/>
+    <d v="2025-04-07T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="7100"/>
+    <d v="2025-09-07T00:00:00"/>
+    <d v="2026-01-18T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="72"/>
+    <d v="2026-04-19T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="2600"/>
+    <d v="2026-07-19T00:00:00"/>
+    <d v="2026-03-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="73"/>
+    <d v="2025-01-01T00:00:00"/>
+    <s v="Marini E."/>
+    <n v="4400"/>
+    <d v="2025-04-01T00:00:00"/>
+    <d v="2026-02-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="74"/>
+    <d v="2025-11-11T00:00:00"/>
+    <s v="Risti"/>
+    <n v="9500"/>
+    <d v="2026-02-11T00:00:00"/>
+    <d v="2025-03-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="75"/>
+    <d v="2025-06-28T00:00:00"/>
+    <s v="Villani"/>
+    <n v="3300"/>
+    <d v="2025-09-28T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="76"/>
+    <d v="2025-08-09T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="1550"/>
+    <d v="2025-11-09T00:00:00"/>
+    <d v="2025-08-25T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="77"/>
+    <d v="2026-02-04T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="5900"/>
+    <d v="2026-05-04T00:00:00"/>
+    <d v="2026-05-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="78"/>
+    <d v="2025-10-18T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="2750"/>
+    <d v="2026-01-18T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="79"/>
+    <d v="2024-12-01T00:00:00"/>
+    <s v="Rossi M."/>
+    <n v="1000"/>
+    <d v="2025-03-01T00:00:00"/>
+    <d v="2026-05-25T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="80"/>
+    <d v="2025-07-23T00:00:00"/>
+    <s v="Lanza C."/>
+    <n v="6800"/>
+    <d v="2025-10-23T00:00:00"/>
+    <d v="2026-03-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="81"/>
+    <d v="2026-04-15T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="1890.5"/>
+    <d v="2026-07-15T00:00:00"/>
+    <d v="2025-10-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="82"/>
+    <d v="2026-03-06T00:00:00"/>
+    <s v="Bianchi R."/>
+    <n v="4100"/>
+    <d v="2026-03-06T00:00:00"/>
+    <d v="2026-03-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="83"/>
+    <d v="2025-06-20T00:00:00"/>
+    <s v="Villani"/>
+    <n v="750"/>
+    <d v="2025-09-20T00:00:00"/>
+    <d v="2025-06-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="84"/>
+    <d v="2026-01-17T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="2980"/>
+    <d v="2026-04-17T00:00:00"/>
+    <d v="2025-07-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="85"/>
+    <d v="2025-08-29T00:00:00"/>
+    <s v="Marini G."/>
+    <n v="1250"/>
+    <d v="2025-11-29T00:00:00"/>
+    <d v="2025-09-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="86"/>
+    <d v="2025-09-14T00:00:00"/>
+    <s v="Risti"/>
+    <n v="9870.2999999999993"/>
+    <d v="2025-12-14T00:00:00"/>
+    <d v="2026-04-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="87"/>
+    <d v="2025-04-08T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="645"/>
+    <d v="2025-07-08T00:00:00"/>
+    <d v="2026-02-25T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="88"/>
+    <d v="2025-11-03T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="3200"/>
+    <d v="2026-02-03T00:00:00"/>
+    <d v="2025-06-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="89"/>
+    <d v="2025-08-24T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="150"/>
+    <d v="2025-11-24T00:00:00"/>
+    <d v="2026-01-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="90"/>
+    <d v="2025-02-10T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="11230"/>
+    <d v="2025-05-10T00:00:00"/>
+    <d v="2026-03-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="91"/>
+    <d v="2026-01-06T00:00:00"/>
+    <s v="Bianchi A."/>
+    <n v="4500"/>
+    <d v="2026-04-06T00:00:00"/>
+    <d v="2026-03-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="92"/>
+    <d v="2025-10-19T00:00:00"/>
+    <s v="Lanza A."/>
+    <n v="7890"/>
+    <d v="2026-01-19T00:00:00"/>
+    <d v="2026-02-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="93"/>
+    <d v="2025-07-01T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="1050"/>
+    <d v="2025-10-01T00:00:00"/>
+    <d v="2026-04-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="94"/>
+    <d v="2025-12-15T00:00:00"/>
+    <s v="Rossi F."/>
+    <n v="3450.9"/>
+    <d v="2026-03-15T00:00:00"/>
+    <d v="2026-03-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="95"/>
+    <d v="2025-05-09T00:00:00"/>
+    <s v="Villani"/>
+    <n v="2150"/>
+    <d v="2025-08-09T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="96"/>
+    <d v="2025-09-04T00:00:00"/>
+    <s v="Marini E."/>
+    <n v="99.5"/>
+    <d v="2025-12-04T00:00:00"/>
+    <d v="2026-01-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="97"/>
+    <d v="2026-04-18T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="12000"/>
+    <d v="2026-07-18T00:00:00"/>
+    <d v="2026-03-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <d v="2025-01-23T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="350"/>
+    <d v="2025-04-23T00:00:00"/>
+    <d v="2026-01-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="99"/>
+    <d v="2025-12-07T00:00:00"/>
+    <s v="Risti"/>
+    <n v="6700"/>
+    <d v="2026-03-07T00:00:00"/>
+    <d v="2025-06-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="100"/>
+    <d v="2026-02-21T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="1450"/>
+    <d v="2026-05-21T00:00:00"/>
+    <d v="2025-09-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="101"/>
+    <d v="2025-07-05T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="8200"/>
+    <d v="2025-10-05T00:00:00"/>
+    <d v="2025-09-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="102"/>
+    <d v="2025-08-29T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="500"/>
+    <d v="2025-11-29T00:00:00"/>
+    <d v="2026-04-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="103"/>
+    <d v="2026-01-11T00:00:00"/>
+    <s v="Lanza C."/>
+    <n v="3750"/>
+    <d v="2026-04-11T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="104"/>
+    <d v="2025-12-14T00:00:00"/>
+    <s v="Villani"/>
+    <n v="2900"/>
+    <d v="2026-03-14T00:00:00"/>
+    <d v="2025-09-24T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="105"/>
+    <d v="2026-02-03T00:00:00"/>
+    <s v="Rossi M."/>
+    <n v="1600"/>
+    <d v="2026-05-03T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="106"/>
+    <d v="2025-06-16T00:00:00"/>
+    <s v="Bianchi R."/>
+    <n v="450"/>
+    <d v="2025-09-16T00:00:00"/>
+    <d v="2026-03-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="107"/>
+    <d v="2025-10-01T00:00:00"/>
+    <s v="Marini G."/>
+    <n v="1830"/>
+    <d v="2026-01-01T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="108"/>
+    <d v="2025-02-27T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="9000"/>
+    <d v="2025-05-27T00:00:00"/>
+    <d v="2026-05-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="109"/>
+    <d v="2025-11-19T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="125"/>
+    <d v="2026-02-19T00:00:00"/>
+    <d v="2025-09-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="110"/>
+    <d v="2025-09-12T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="5100"/>
+    <d v="2025-12-12T00:00:00"/>
+    <d v="2025-08-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="111"/>
+    <d v="2025-01-08T00:00:00"/>
+    <s v="Risti"/>
+    <n v="1100"/>
+    <d v="2025-04-08T00:00:00"/>
+    <d v="2026-05-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="112"/>
+    <d v="2025-06-04T00:00:00"/>
+    <s v="Villani"/>
+    <n v="15000"/>
+    <d v="2025-09-04T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="77"/>
+  </r>
+  <r>
+    <n v="113"/>
+    <d v="2026-04-21T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="2340"/>
+    <d v="2026-07-21T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="114"/>
+    <d v="2026-03-15T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="7900"/>
+    <d v="2026-06-15T00:00:00"/>
+    <d v="2025-12-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="115"/>
+    <d v="2025-08-03T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="400"/>
+    <d v="2025-11-03T00:00:00"/>
+    <d v="2026-04-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="116"/>
+    <d v="2025-12-28T00:00:00"/>
+    <s v="Lanza A."/>
+    <n v="1700"/>
+    <d v="2026-03-28T00:00:00"/>
+    <d v="2025-06-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="117"/>
+    <d v="2025-10-09T00:00:00"/>
+    <s v="Rossi F."/>
+    <n v="5600"/>
+    <d v="2026-01-09T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="118"/>
+    <d v="2026-02-20T00:00:00"/>
+    <s v="Bianchi A."/>
+    <n v="9200"/>
+    <d v="2026-05-20T00:00:00"/>
+    <d v="2025-11-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="119"/>
+    <d v="2025-04-01T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="3100"/>
+    <d v="2025-07-01T00:00:00"/>
+    <d v="2026-03-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="120"/>
+    <d v="2026-01-14T00:00:00"/>
+    <s v="Marini E."/>
+    <n v="1200"/>
+    <d v="2026-04-14T00:00:00"/>
+    <d v="2025-07-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="121"/>
+    <d v="2025-11-26T00:00:00"/>
+    <s v="Villani"/>
+    <n v="800"/>
+    <d v="2026-02-26T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="122"/>
+    <d v="2025-09-10T00:00:00"/>
+    <s v="Risti"/>
+    <n v="5500"/>
+    <d v="2025-12-10T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="123"/>
+    <d v="2026-01-05T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="12500"/>
+    <d v="2026-04-05T00:00:00"/>
+    <d v="2026-05-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="124"/>
+    <d v="2025-08-23T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="4800"/>
+    <d v="2025-11-23T00:00:00"/>
+    <d v="2025-08-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="125"/>
+    <d v="2025-12-17T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="1950"/>
+    <d v="2026-03-17T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="126"/>
+    <d v="2025-06-19T00:00:00"/>
+    <s v="Lanza C."/>
+    <n v="6000"/>
+    <d v="2025-09-19T00:00:00"/>
+    <d v="2025-12-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="127"/>
+    <d v="2024-12-08T00:00:00"/>
+    <s v="Rossi M."/>
+    <n v="300"/>
+    <d v="2025-03-08T00:00:00"/>
+    <d v="2026-02-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="128"/>
+    <d v="2025-11-02T00:00:00"/>
+    <s v="Bianchi R."/>
+    <n v="250"/>
+    <d v="2026-02-02T00:00:00"/>
+    <d v="2026-03-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="129"/>
+    <d v="2026-01-20T00:00:00"/>
+    <s v="Villani"/>
+    <n v="8800"/>
+    <d v="2026-04-20T00:00:00"/>
+    <d v="2026-07-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="130"/>
+    <d v="2025-04-06T00:00:00"/>
+    <s v="Marini G."/>
+    <n v="1100"/>
+    <d v="2025-07-06T00:00:00"/>
+    <d v="2026-04-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="131"/>
+    <d v="2026-02-13T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="4300"/>
+    <d v="2026-05-13T00:00:00"/>
+    <d v="2026-05-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="132"/>
+    <d v="2025-10-18T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="900"/>
+    <d v="2026-01-18T00:00:00"/>
+    <d v="2026-03-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="133"/>
+    <d v="2025-07-24T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="1750"/>
+    <d v="2025-10-24T00:00:00"/>
+    <d v="2025-06-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="134"/>
+    <d v="2026-01-07T00:00:00"/>
+    <s v="Risti"/>
+    <n v="2900"/>
+    <d v="2026-04-07T00:00:00"/>
+    <d v="2026-01-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="135"/>
+    <d v="2025-12-29T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="6200"/>
+    <d v="2026-03-29T00:00:00"/>
+    <d v="2025-11-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="136"/>
+    <d v="2025-08-10T00:00:00"/>
+    <s v="Lanza A."/>
+    <n v="3600"/>
+    <d v="2025-11-10T00:00:00"/>
+    <d v="2026-03-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="137"/>
+    <d v="2026-02-04T00:00:00"/>
+    <s v="Rossi F."/>
+    <n v="1500"/>
+    <d v="2026-05-04T00:00:00"/>
+    <d v="2026-05-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="138"/>
+    <d v="2025-09-12T00:00:00"/>
+    <s v="Bianchi A."/>
+    <n v="4900"/>
+    <d v="2026-03-12T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="139"/>
+    <d v="2025-03-01T00:00:00"/>
+    <s v="Villani"/>
+    <n v="2100"/>
+    <d v="2025-06-01T00:00:00"/>
+    <d v="2026-01-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="140"/>
+    <d v="2025-08-17T00:00:00"/>
+    <s v="Marini E."/>
+    <n v="7300"/>
+    <d v="2025-11-17T00:00:00"/>
+    <d v="2026-03-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="141"/>
+    <d v="2025-05-21T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="180"/>
+    <d v="2025-08-21T00:00:00"/>
+    <d v="2025-07-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="142"/>
+    <d v="2025-10-15T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="5400"/>
+    <d v="2026-01-15T00:00:00"/>
+    <d v="2026-03-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="143"/>
+    <d v="2026-04-28T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="1350"/>
+    <d v="2026-07-28T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="144"/>
+    <d v="2025-02-03T00:00:00"/>
+    <s v="Risti"/>
+    <n v="9800"/>
+    <d v="2025-05-03T00:00:00"/>
+    <d v="2026-05-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="145"/>
+    <d v="2025-07-16T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="450"/>
+    <d v="2025-10-16T00:00:00"/>
+    <d v="2026-05-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="146"/>
+    <d v="2025-11-08T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="2700"/>
+    <d v="2026-02-08T00:00:00"/>
+    <d v="2026-05-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="147"/>
+    <d v="2025-09-23T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="6500"/>
+    <d v="2025-12-23T00:00:00"/>
+    <d v="2026-03-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="148"/>
+    <d v="2025-12-11T00:00:00"/>
+    <s v="Lanza C."/>
+    <n v="3900"/>
+    <d v="2026-03-11T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="149"/>
+    <d v="2026-04-20T00:00:00"/>
+    <s v="Villani"/>
+    <n v="8100"/>
+    <d v="2026-07-20T00:00:00"/>
+    <d v="2026-03-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="150"/>
+    <d v="2025-06-05T00:00:00"/>
+    <s v="Rossi M."/>
+    <n v="12000"/>
+    <d v="2025-09-05T00:00:00"/>
+    <d v="2025-09-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="151"/>
+    <d v="2026-01-17T00:00:00"/>
+    <s v="Bianchi R."/>
+    <n v="2200"/>
+    <d v="2026-04-17T00:00:00"/>
+    <d v="2025-05-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="152"/>
+    <d v="2026-02-12T00:00:00"/>
+    <s v="Marini G."/>
+    <n v="1400"/>
+    <d v="2026-05-12T00:00:00"/>
+    <d v="2026-03-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="153"/>
+    <d v="2025-05-25T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="7700"/>
+    <d v="2025-08-25T00:00:00"/>
+    <d v="2025-05-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="154"/>
+    <d v="2025-12-10T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="3500"/>
+    <d v="2026-03-10T00:00:00"/>
+    <d v="2025-09-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="155"/>
+    <d v="2025-02-01T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="9000"/>
+    <d v="2025-05-01T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="203"/>
+  </r>
+  <r>
+    <n v="156"/>
+    <d v="2025-06-15T00:00:00"/>
+    <s v="Risti"/>
+    <n v="1600"/>
+    <d v="2025-09-15T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="66"/>
+  </r>
+  <r>
+    <n v="157"/>
+    <d v="2025-08-05T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="4600"/>
+    <d v="2025-11-05T00:00:00"/>
+    <d v="2025-04-25T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="158"/>
+    <d v="2026-04-20T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="550"/>
+    <d v="2026-07-20T00:00:00"/>
+    <d v="2026-01-25T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="159"/>
+    <d v="2025-01-11T00:00:00"/>
+    <s v="Villani"/>
+    <n v="10500"/>
+    <d v="2025-04-11T00:00:00"/>
+    <d v="2025-03-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="160"/>
+    <d v="2025-10-03T00:00:00"/>
+    <s v="Lanza A."/>
+    <n v="2500"/>
+    <d v="2026-01-03T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="161"/>
+    <d v="2024-12-18T00:00:00"/>
+    <s v="Rossi F."/>
+    <n v="1900"/>
+    <d v="2025-03-18T00:00:00"/>
+    <d v="2025-05-05T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="162"/>
+    <d v="2025-11-02T00:00:00"/>
+    <s v="Bianchi A."/>
+    <n v="8400"/>
+    <d v="2026-02-02T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="163"/>
+    <d v="2025-01-29T00:00:00"/>
+    <s v="Marini E."/>
+    <n v="3200"/>
+    <d v="2025-04-29T00:00:00"/>
+    <d v="2025-08-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="164"/>
+    <d v="2025-09-14T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="4700"/>
+    <d v="2025-12-14T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="165"/>
+    <d v="2025-04-08T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="1150"/>
+    <d v="2025-07-08T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="135"/>
+  </r>
+  <r>
+    <n v="166"/>
+    <d v="2025-10-22T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="5300"/>
+    <d v="2026-01-22T00:00:00"/>
+    <d v="2025-06-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="167"/>
+    <d v="2026-01-17T00:00:00"/>
+    <s v="Risti"/>
+    <n v="15000"/>
+    <d v="2026-04-17T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="168"/>
+    <d v="2025-03-06T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="650"/>
+    <d v="2025-06-06T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="167"/>
+  </r>
+  <r>
+    <n v="169"/>
+    <d v="2025-12-09T00:00:00"/>
+    <s v="Villani"/>
+    <n v="2800"/>
+    <d v="2026-03-09T00:00:00"/>
+    <d v="2025-04-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="170"/>
+    <d v="2025-11-19T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="1850"/>
+    <d v="2026-02-19T00:00:00"/>
+    <d v="2025-11-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="171"/>
+    <d v="2025-01-21T00:00:00"/>
+    <s v="Lanza C."/>
+    <n v="7100"/>
+    <d v="2025-04-21T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="213"/>
+  </r>
+  <r>
+    <n v="172"/>
+    <d v="2025-07-04T00:00:00"/>
+    <s v="Rossi M."/>
+    <n v="2600"/>
+    <d v="2025-10-04T00:00:00"/>
+    <d v="2026-01-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="173"/>
+    <d v="2025-12-07T00:00:00"/>
+    <s v="Bianchi R."/>
+    <n v="4400"/>
+    <d v="2026-03-07T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="174"/>
+    <d v="2025-09-23T00:00:00"/>
+    <s v="Marini G."/>
+    <n v="9500"/>
+    <d v="2025-12-23T00:00:00"/>
+    <d v="2025-07-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="175"/>
+    <d v="2026-02-13T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="3300"/>
+    <d v="2026-05-13T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="176"/>
+    <d v="2025-04-01T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="1550"/>
+    <d v="2025-07-01T00:00:00"/>
+    <d v="2025-06-05T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="177"/>
+    <d v="2025-12-17T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="5900"/>
+    <d v="2026-03-17T00:00:00"/>
+    <d v="2025-11-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="178"/>
+    <d v="2025-02-28T00:00:00"/>
+    <s v="Risti"/>
+    <n v="2750"/>
+    <d v="2025-05-28T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="176"/>
+  </r>
+  <r>
+    <n v="179"/>
+    <d v="2025-08-02T00:00:00"/>
+    <s v="Villani"/>
+    <n v="1000"/>
+    <d v="2025-11-02T00:00:00"/>
+    <d v="2025-04-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="180"/>
+    <d v="2025-10-11T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="6800"/>
+    <d v="2026-01-11T00:00:00"/>
+    <d v="2025-06-10T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="181"/>
+    <d v="2025-01-04T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="1890.5"/>
+    <d v="2025-04-04T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="230"/>
+  </r>
+  <r>
+    <n v="182"/>
+    <d v="2025-03-16T00:00:00"/>
+    <s v="Lanza A."/>
+    <n v="4100"/>
+    <d v="2025-06-16T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="157"/>
+  </r>
+  <r>
+    <n v="183"/>
+    <d v="2025-11-27T00:00:00"/>
+    <s v="Pinca V."/>
+    <n v="750"/>
+    <d v="2026-02-27T00:00:00"/>
+    <d v="2025-10-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="184"/>
+    <d v="2026-01-12T00:00:00"/>
+    <s v="Rossi F."/>
+    <n v="2980"/>
+    <d v="2026-04-12T00:00:00"/>
+    <d v="2025-03-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="185"/>
+    <d v="2025-06-05T00:00:00"/>
+    <s v="Bianchi A."/>
+    <n v="1250"/>
+    <d v="2025-09-05T00:00:00"/>
+    <d v="2025-11-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="186"/>
+    <d v="2024-12-20T00:00:00"/>
+    <s v="Marini E."/>
+    <n v="9870.2999999999993"/>
+    <d v="2025-03-20T00:00:00"/>
+    <d v="2025-09-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="187"/>
+    <d v="2025-08-13T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="645"/>
+    <d v="2025-11-13T00:00:00"/>
+    <d v="2025-11-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="188"/>
+    <d v="2025-05-09T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="3200"/>
+    <d v="2025-08-09T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="103"/>
+  </r>
+  <r>
+    <n v="189"/>
+    <d v="2025-07-24T00:00:00"/>
+    <s v="Risti"/>
+    <n v="150"/>
+    <d v="2025-10-24T00:00:00"/>
+    <d v="2025-03-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="190"/>
+    <d v="2026-02-03T00:00:00"/>
+    <s v="Villani"/>
+    <n v="11230"/>
+    <d v="2026-05-03T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="191"/>
+    <d v="2024-12-15T00:00:00"/>
+    <s v="Fornari"/>
+    <n v="4500"/>
+    <d v="2025-03-15T00:00:00"/>
+    <d v="2025-12-15T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="192"/>
+    <d v="2025-10-21T00:00:00"/>
+    <s v="Trefoloni"/>
+    <n v="7890"/>
+    <d v="2026-01-21T00:00:00"/>
+    <d v="2025-09-05T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="193"/>
+    <d v="2025-09-10T00:00:00"/>
+    <s v="Lanza C."/>
+    <n v="1050"/>
+    <d v="2025-12-10T00:00:00"/>
+    <d v="2025-06-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="194"/>
+    <d v="2025-05-28T00:00:00"/>
+    <s v="Rossi M."/>
+    <n v="3450.9"/>
+    <d v="2025-08-28T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="84"/>
+  </r>
+  <r>
+    <n v="195"/>
+    <d v="2025-03-01T00:00:00"/>
+    <s v="Bianchi R."/>
+    <n v="2150"/>
+    <d v="2025-06-01T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="2"/>
+    <n v="172"/>
+  </r>
+  <r>
+    <n v="196"/>
+    <d v="2026-01-07T00:00:00"/>
+    <s v="Marini G."/>
+    <n v="99.5"/>
+    <d v="2026-04-07T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="197"/>
+    <d v="2026-02-26T00:00:00"/>
+    <s v="Pinca S."/>
+    <n v="12000"/>
+    <d v="2026-05-26T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="198"/>
+    <d v="2025-11-19T00:00:00"/>
+    <s v="Sereni"/>
+    <n v="350"/>
+    <d v="2026-02-19T00:00:00"/>
+    <d v="2025-11-01T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="199"/>
+    <d v="2025-12-14T00:00:00"/>
+    <s v="Scottà"/>
+    <n v="6700"/>
+    <d v="2026-03-14T00:00:00"/>
+    <m/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="200"/>
+    <d v="2025-07-20T00:00:00"/>
+    <s v="Risti"/>
+    <n v="1450"/>
+    <d v="2025-10-20T00:00:00"/>
+    <d v="2025-09-20T00:00:00"/>
+    <d v="2025-11-20T00:00:00"/>
+    <x v="0"/>
+    <n v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{196B16F7-4DED-4405-8DBA-D4AF07510499}" name="Tabella pivot1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Calculated Status">
+  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Invoice Number" fld="0" subtotal="count" baseField="7" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="0" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4665,8 +8427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD82BC1-84A4-4280-BEAB-AE99592285DD}">
   <dimension ref="A1:I201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
@@ -10822,7 +14584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A164D69F-5719-4ECE-A976-CD9A45525F6C}">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -10845,14 +14607,14 @@
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="G2" s="20" t="s">
+      <c r="D2" s="23"/>
+      <c r="G2" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="21"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -10894,11 +14656,11 @@
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="23" t="str">
+      <c r="D5" s="20" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D4)</f>
         <v>=CONTA.SE(Analysis_Sheet!C:C; Dashboard!C4)</v>
       </c>
-      <c r="H5" s="22" t="str">
+      <c r="H5" s="20" t="str">
         <f ca="1">_xlfn.FORMULATEXT(H4)</f>
         <v>=CONTA.PIÙ.SE(Analysis_Sheet!C:C; G4; Analysis_Sheet!H:H; "Overdue") + CONTA.PIÙ.SE(Analysis_Sheet!C:C; G4; Analysis_Sheet!H:H; "Unpaid")</v>
       </c>
@@ -10922,14 +14684,14 @@
       <c r="A9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="G9" s="20" t="s">
+      <c r="D9" s="23"/>
+      <c r="G9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="21"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
@@ -10971,11 +14733,11 @@
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="23" t="str">
+      <c r="D12" s="20" t="str">
         <f ca="1">_xlfn.FORMULATEXT(D11)</f>
         <v>=SOMMA.SE(Analysis_Sheet!C:C;C11; Analysis_Sheet!D:D )</v>
       </c>
-      <c r="H12" s="24" t="str">
+      <c r="H12" s="21" t="str">
         <f ca="1">_xlfn.FORMULATEXT(H11)</f>
         <v>=SOMMA.PIÙ.SE(Analysis_Sheet!D:D; Analysis_Sheet!C:C; G11; Analysis_Sheet!H:H; "Overdue") + SOMMA.PIÙ.SE(Analysis_Sheet!D:D; Analysis_Sheet!C:C; G11; Analysis_Sheet!H:H; "Unpaid")</v>
       </c>
@@ -11571,4 +15333,64 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D593E3-7876-49B2-AB89-4C24A8E228CA}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="25">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FEAT & DOCS: Complete Report 2 (Monetary Exposure) and update README
Adds Pivot Table 2 (Total Amount by Status) and Chart 2 (3D Column Chart) to the Reporting sheet. Documents the new analysis in Section 8 of the README. Includes the final assets: screenshot_8 (setup) and screenshot_9 (clean chart).
</commit_message>
<xml_diff>
--- a/Customer_Invoice_Analysis - filled.xlsx
+++ b/Customer_Invoice_Analysis - filled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\invoice-analysis-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721774B7-958E-4149-A890-92053AAA32D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFB992F-0874-48E9-80B1-22FE9F2A8CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{56643878-06B9-462D-81B7-435828026F01}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="38">
   <si>
     <t>Sereni</t>
   </si>
@@ -160,7 +160,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
@@ -396,14 +397,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Colore 3" xfId="5" builtinId="39"/>
@@ -555,7 +556,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1241,7 +1242,982 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Customer_Invoice_Analysis - filled.xlsx]Reporting!Tabella pivot2</c:name>
+    <c:fmtId val="7"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Total Amount by Status</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="4.0380047505938155E-2"/>
+              <c:y val="-2.9850746268656716E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:fld id="{A0942BA4-0C50-4C5A-A197-3A03DA618864}" type="VALUE">
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:pPr>
+                    <a:defRPr/>
+                  </a:pPr>
+                  <a:t>[VALORE]</a:t>
+                </a:fld>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:dlblFieldTable/>
+              <c15:showDataLabelsRange val="0"/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="2.8503562945368172E-2"/>
+              <c:y val="-3.7313432835820892E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:fld id="{E4A24557-3CD7-4588-A9F7-722907E42AB2}" type="VALUE">
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:pPr>
+                    <a:defRPr/>
+                  </a:pPr>
+                  <a:t>[VALORE]</a:t>
+                </a:fld>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:dlblFieldTable/>
+              <c15:showDataLabelsRange val="0"/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+          <a:sp3d/>
+        </c:spPr>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="3.0878859857482184E-2"/>
+              <c:y val="-5.2238805970149252E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:fld id="{883E96BF-0F40-4B6D-A449-9905BEA67D24}" type="VALUE">
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:pPr>
+                    <a:defRPr/>
+                  </a:pPr>
+                  <a:t>[VALORE]</a:t>
+                </a:fld>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+              <c15:dlblFieldTable/>
+              <c15:showDataLabelsRange val="0"/>
+            </c:ext>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reporting!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Totale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-EF11-47A1-A1B7-BB56E86EE4FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-EF11-47A1-A1B7-BB56E86EE4FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-EF11-47A1-A1B7-BB56E86EE4FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.8503562945368172E-2"/>
+                  <c:y val="-3.7313432835820892E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E4A24557-3CD7-4588-A9F7-722907E42AB2}" type="VALUE">
+                      <a:rPr lang="en-US" b="1"/>
+                      <a:pPr/>
+                      <a:t>[VALORE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-EF11-47A1-A1B7-BB56E86EE4FD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.0878859857482184E-2"/>
+                  <c:y val="-5.2238805970149252E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{883E96BF-0F40-4B6D-A449-9905BEA67D24}" type="VALUE">
+                      <a:rPr lang="en-US" b="1"/>
+                      <a:pPr/>
+                      <a:t>[VALORE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-EF11-47A1-A1B7-BB56E86EE4FD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.0380047505938155E-2"/>
+                  <c:y val="-2.9850746268656716E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A0942BA4-0C50-4C5A-A197-3A03DA618864}" type="VALUE">
+                      <a:rPr lang="en-US" b="1"/>
+                      <a:pPr/>
+                      <a:t>[VALORE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="it-IT"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-EF11-47A1-A1B7-BB56E86EE4FD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Reporting!$M$2:$M$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Overdue</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Paid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unpaid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reporting!$N$2:$N$5</c:f>
+              <c:numCache>
+                <c:formatCode>"€"#,##0.00_);\("€"#,##0.00\)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>59063.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>601412.84000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164252.51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EF11-47A1-A1B7-BB56E86EE4FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="478361055"/>
+        <c:axId val="480384495"/>
+        <c:axId val="0"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="478361055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="480384495"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="480384495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;€&quot;#,##0.00_);\(&quot;€&quot;#,##0.00\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="478361055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1800,6 +2776,500 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1833,6 +3303,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C4EF033-D22F-8CB2-36E4-B2FD443DC544}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4093,7 +5599,110 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{196B16F7-4DED-4405-8DBA-D4AF07510499}" name="Tabella pivot1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Calculated Status">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9AF67EA-B7F4-48A0-B9DF-28596B9CC96C}" name="Tabella pivot2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13" rowHeaderCaption="Calculated Status">
+  <location ref="M1:N5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Total Amount" fld="3" baseField="7" baseItem="0" numFmtId="7"/>
+  </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="7" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="7" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="0" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{196B16F7-4DED-4405-8DBA-D4AF07510499}" name="Tabella pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Calculated Status">
   <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0"/>
@@ -14607,14 +16216,14 @@
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="G2" s="22" t="s">
+      <c r="D2" s="25"/>
+      <c r="G2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="23"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -14684,14 +16293,14 @@
       <c r="A9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="G9" s="22" t="s">
+      <c r="D9" s="25"/>
+      <c r="G9" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="23"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
@@ -15337,60 +16946,92 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D593E3-7876-49B2-AB89-4C24A8E228CA}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="M1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="M2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="23">
+        <v>59063.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="M3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="23">
+        <v>601412.84000000008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="M4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="23">
+        <v>164252.51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5">
         <v>200</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="23">
+        <v>824728.75000000012</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
renamed screenshot 8 and 9
</commit_message>
<xml_diff>
--- a/Customer_Invoice_Analysis - filled.xlsx
+++ b/Customer_Invoice_Analysis - filled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\invoice-analysis-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFB992F-0874-48E9-80B1-22FE9F2A8CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609D49F2-2C8D-4602-B93B-B7CE2FEBF34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{56643878-06B9-462D-81B7-435828026F01}"/>
   </bookViews>
@@ -16949,7 +16949,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
feat: Complete Customer Revenue Ranking Chart and README Documentation
This commit finalizes the third key analysis chart and updates the project documentation:

* Implemented and formatted Pivot Table 3 and the associated Horizontal Bar Chart ('Customer Revenue Ranking').
* Applied advanced chart formatting (axis reversal, currency format) to correctly display customer ranking from highest to lowest revenue.
* Added comprehensive documentation for Section 9 in README.md (in English), focusing on 'Customer Concentration Risk Analysis'.
* Included references and captions for two new required screenshots (screenshot_10 and screenshot_11).
</commit_message>
<xml_diff>
--- a/Customer_Invoice_Analysis - filled.xlsx
+++ b/Customer_Invoice_Analysis - filled.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\invoice-analysis-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609D49F2-2C8D-4602-B93B-B7CE2FEBF34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C7B82D-312E-45A9-A5F2-858FD1880813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{56643878-06B9-462D-81B7-435828026F01}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{56643878-06B9-462D-81B7-435828026F01}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice_Master_Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="39">
   <si>
     <t>Sereni</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Invoice Total</t>
   </si>
 </sst>
 </file>
@@ -334,7 +337,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -405,6 +408,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Colore 3" xfId="5" builtinId="39"/>
@@ -443,6 +447,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFFFF"/>
       <color rgb="FFFF3333"/>
       <color rgb="FF72AF2F"/>
       <color rgb="FF85CA3A"/>
@@ -2177,6 +2182,540 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Customer_Invoice_Analysis - filled.xlsx]Reporting!Tabella pivot3</c:name>
+    <c:fmtId val="3"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Total Amount by Customer</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Reporting!$AA$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Totale</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Reporting!$Z$2:$Z$18</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Risti</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Villani</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sereni</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Pinca S.</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bianchi A.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Scottà</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Trefoloni</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Marini E.</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lanza A.</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Fornari</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Pinca V.</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Lanza C.</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Rossi F.</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Rossi M.</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Bianchi R.</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Marini G.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Reporting!$AA$2:$AA$18</c:f>
+              <c:numCache>
+                <c:formatCode>_-"€"* #,##0.00_-;\-"€"* #,##0.00_-;_-"€"* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>87093.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84414</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76889.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63524</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62450</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61494.36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55903.979999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51475.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48792.619999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48190</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44341.479999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37947.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33615.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28290.74</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23166.67</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17139.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F07B-4B3D-AFAA-49FFEDA15BF1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1871606383"/>
+        <c:axId val="1871593903"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1871606383"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1871593903"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1871593903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00\ &quot;€&quot;" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-1800000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1871606383"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2218,6 +2757,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3270,6 +3849,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3344,6 +4428,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>88653</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>56490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>279153</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>139041</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Grafico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44642112-27CE-7FC2-EBC6-7996FB8FDF63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3360,7 +4480,24 @@
       <sharedItems containsDate="1" containsMixedTypes="1" minDate="2024-09-12T00:00:00" maxDate="2026-04-29T00:00:00"/>
     </cacheField>
     <cacheField name="Customer" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="16">
+        <s v="Rossi M."/>
+        <s v="Pinca S."/>
+        <s v="Sereni"/>
+        <s v="Scottà"/>
+        <s v="Villani"/>
+        <s v="Bianchi R."/>
+        <s v="Lanza A."/>
+        <s v="Trefoloni"/>
+        <s v="Pinca V."/>
+        <s v="Risti"/>
+        <s v="Rossi F."/>
+        <s v="Bianchi A."/>
+        <s v="Fornari"/>
+        <s v="Lanza C."/>
+        <s v="Marini E."/>
+        <s v="Marini G."/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Amount" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="60" maxValue="23456"/>
@@ -3398,7 +4535,7 @@
   <r>
     <n v="1"/>
     <d v="2025-05-25T00:00:00"/>
-    <s v="Rossi M."/>
+    <x v="0"/>
     <n v="450"/>
     <d v="2025-08-25T00:00:00"/>
     <d v="2025-08-20T00:00:00"/>
@@ -3409,7 +4546,7 @@
   <r>
     <n v="2"/>
     <d v="2025-12-10T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="3562"/>
     <d v="2026-03-10T00:00:00"/>
     <m/>
@@ -3420,7 +4557,7 @@
   <r>
     <n v="3"/>
     <d v="2025-02-01T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="2700"/>
     <d v="2025-05-01T00:00:00"/>
     <d v="2025-05-15T00:00:00"/>
@@ -3431,7 +4568,7 @@
   <r>
     <n v="4"/>
     <d v="2025-06-15T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="399.36"/>
     <d v="2025-09-15T00:00:00"/>
     <d v="2025-10-05T00:00:00"/>
@@ -3442,7 +4579,7 @@
   <r>
     <n v="5"/>
     <d v="2025-08-05T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="960"/>
     <d v="2025-11-05T00:00:00"/>
     <m/>
@@ -3453,7 +4590,7 @@
   <r>
     <n v="6"/>
     <d v="2026-04-20T00:00:00"/>
-    <s v="Bianchi R."/>
+    <x v="5"/>
     <n v="7916.67"/>
     <d v="2026-07-20T00:00:00"/>
     <m/>
@@ -3464,7 +4601,7 @@
   <r>
     <n v="7"/>
     <d v="2025-01-11T00:00:00"/>
-    <s v="Lanza A."/>
+    <x v="6"/>
     <n v="3360"/>
     <d v="2025-04-11T00:00:00"/>
     <d v="2025-05-11T00:00:00"/>
@@ -3475,7 +4612,7 @@
   <r>
     <n v="8"/>
     <d v="2025-10-03T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="1839.36"/>
     <d v="2026-01-03T00:00:00"/>
     <m/>
@@ -3486,7 +4623,7 @@
   <r>
     <n v="9"/>
     <d v="2024-12-18T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="477.48"/>
     <d v="2025-03-18T00:00:00"/>
     <d v="2025-03-20T00:00:00"/>
@@ -3497,7 +4634,7 @@
   <r>
     <n v="10"/>
     <d v="2025-11-02T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="750"/>
     <d v="2026-02-02T00:00:00"/>
     <m/>
@@ -3508,7 +4645,7 @@
   <r>
     <n v="11"/>
     <d v="2025-01-29T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="750"/>
     <d v="2025-04-29T00:00:00"/>
     <d v="2025-05-05T00:00:00"/>
@@ -3519,7 +4656,7 @@
   <r>
     <n v="12"/>
     <d v="2025-09-14T00:00:00"/>
-    <s v="Rossi F."/>
+    <x v="10"/>
     <n v="3284.5"/>
     <d v="2025-12-14T00:00:00"/>
     <m/>
@@ -3530,7 +4667,7 @@
   <r>
     <n v="13"/>
     <d v="2025-04-08T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="4320"/>
     <d v="2025-07-08T00:00:00"/>
     <d v="2025-08-01T00:00:00"/>
@@ -3541,7 +4678,7 @@
   <r>
     <n v="14"/>
     <d v="2025-10-22T00:00:00"/>
-    <s v="Bianchi A."/>
+    <x v="11"/>
     <n v="9600"/>
     <d v="2026-01-22T00:00:00"/>
     <m/>
@@ -3552,7 +4689,7 @@
   <r>
     <n v="15"/>
     <d v="2026-01-17T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="234"/>
     <d v="2026-04-17T00:00:00"/>
     <m/>
@@ -3563,7 +4700,7 @@
   <r>
     <n v="16"/>
     <d v="2025-03-06T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="12000"/>
     <d v="2025-06-06T00:00:00"/>
     <d v="2025-06-10T00:00:00"/>
@@ -3574,7 +4711,7 @@
   <r>
     <n v="17"/>
     <d v="2025-12-09T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="123"/>
     <d v="2026-03-09T00:00:00"/>
     <m/>
@@ -3585,7 +4722,7 @@
   <r>
     <n v="18"/>
     <d v="2025-11-19T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="790"/>
     <d v="2026-02-19T00:00:00"/>
     <m/>
@@ -3596,7 +4733,7 @@
   <r>
     <n v="19"/>
     <d v="2025-01-21T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="580"/>
     <d v="2025-04-21T00:00:00"/>
     <d v="2025-04-20T00:00:00"/>
@@ -3607,7 +4744,7 @@
   <r>
     <n v="20"/>
     <d v="2025-07-04T00:00:00"/>
-    <s v="Lanza C."/>
+    <x v="13"/>
     <n v="2112.6"/>
     <d v="2025-10-04T00:00:00"/>
     <d v="2025-11-01T00:00:00"/>
@@ -3618,7 +4755,7 @@
   <r>
     <n v="21"/>
     <d v="2025-12-07T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="1980"/>
     <d v="2026-03-07T00:00:00"/>
     <m/>
@@ -3629,7 +4766,7 @@
   <r>
     <n v="22"/>
     <d v="2025-09-23T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="534"/>
     <d v="2025-12-23T00:00:00"/>
     <d v="2026-01-01T00:00:00"/>
@@ -3640,7 +4777,7 @@
   <r>
     <n v="23"/>
     <d v="2026-02-13T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="8600"/>
     <d v="2026-05-13T00:00:00"/>
     <m/>
@@ -3651,7 +4788,7 @@
   <r>
     <n v="24"/>
     <d v="2025-04-01T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="1600"/>
     <d v="2025-07-01T00:00:00"/>
     <d v="2025-07-15T00:00:00"/>
@@ -3662,7 +4799,7 @@
   <r>
     <n v="25"/>
     <d v="2025-12-17T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="1050"/>
     <d v="2026-03-17T00:00:00"/>
     <m/>
@@ -3673,7 +4810,7 @@
   <r>
     <n v="26"/>
     <d v="2025-02-28T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="4100"/>
     <d v="2025-05-28T00:00:00"/>
     <d v="2025-06-05T00:00:00"/>
@@ -3684,7 +4821,7 @@
   <r>
     <n v="27"/>
     <d v="2025-08-02T00:00:00"/>
-    <s v="Lanza A."/>
+    <x v="6"/>
     <n v="20112.62"/>
     <d v="2025-11-02T00:00:00"/>
     <d v="2025-11-10T00:00:00"/>
@@ -3695,7 +4832,7 @@
   <r>
     <n v="28"/>
     <d v="2025-10-11T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="1450"/>
     <d v="2026-01-11T00:00:00"/>
     <m/>
@@ -3706,7 +4843,7 @@
   <r>
     <n v="29"/>
     <d v="2025-01-04T00:00:00"/>
-    <s v="Marini E."/>
+    <x v="14"/>
     <n v="23456"/>
     <d v="2025-04-04T00:00:00"/>
     <d v="2025-04-20T00:00:00"/>
@@ -3717,7 +4854,7 @@
   <r>
     <n v="30"/>
     <d v="2025-03-16T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="400"/>
     <d v="2025-06-16T00:00:00"/>
     <d v="2025-06-10T00:00:00"/>
@@ -3728,7 +4865,7 @@
   <r>
     <n v="31"/>
     <d v="2025-11-27T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="750"/>
     <d v="2026-02-27T00:00:00"/>
     <m/>
@@ -3739,7 +4876,7 @@
   <r>
     <n v="32"/>
     <d v="2026-01-12T00:00:00"/>
-    <s v="Lanza C."/>
+    <x v="13"/>
     <n v="3400"/>
     <d v="2026-04-12T00:00:00"/>
     <m/>
@@ -3750,7 +4887,7 @@
   <r>
     <n v="33"/>
     <d v="2025-06-05T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="1560"/>
     <d v="2025-09-05T00:00:00"/>
     <d v="2025-10-01T00:00:00"/>
@@ -3761,7 +4898,7 @@
   <r>
     <n v="34"/>
     <d v="2024-12-20T00:00:00"/>
-    <s v="Rossi M."/>
+    <x v="0"/>
     <n v="2100"/>
     <d v="2025-03-20T00:00:00"/>
     <d v="2025-03-20T00:00:00"/>
@@ -3772,7 +4909,7 @@
   <r>
     <n v="35"/>
     <d v="2025-08-13T00:00:00"/>
-    <s v="Bianchi A."/>
+    <x v="11"/>
     <n v="9600"/>
     <d v="2025-11-13T00:00:00"/>
     <d v="2025-11-15T00:00:00"/>
@@ -3783,7 +4920,7 @@
   <r>
     <n v="36"/>
     <d v="2025-05-09T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="4259.9399999999996"/>
     <d v="2025-08-09T00:00:00"/>
     <d v="2025-09-15T00:00:00"/>
@@ -3794,7 +4931,7 @@
   <r>
     <n v="37"/>
     <d v="2025-07-24T00:00:00"/>
-    <s v="Lanza A."/>
+    <x v="6"/>
     <n v="230"/>
     <d v="2025-10-24T00:00:00"/>
     <d v="2025-11-01T00:00:00"/>
@@ -3805,7 +4942,7 @@
   <r>
     <n v="38"/>
     <d v="2026-02-03T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="3200"/>
     <d v="2026-05-03T00:00:00"/>
     <m/>
@@ -3816,7 +4953,7 @@
   <r>
     <n v="39"/>
     <d v="2024-12-15T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="6780"/>
     <d v="2025-03-15T00:00:00"/>
     <d v="2025-03-20T00:00:00"/>
@@ -3827,7 +4964,7 @@
   <r>
     <n v="40"/>
     <d v="2025-10-21T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="477.48"/>
     <d v="2026-01-21T00:00:00"/>
     <m/>
@@ -3838,7 +4975,7 @@
   <r>
     <n v="41"/>
     <d v="2025-09-10T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="2900"/>
     <d v="2025-12-10T00:00:00"/>
     <d v="2025-12-15T00:00:00"/>
@@ -3849,7 +4986,7 @@
   <r>
     <n v="42"/>
     <d v="2025-05-28T00:00:00"/>
-    <s v="Marini G."/>
+    <x v="15"/>
     <n v="60"/>
     <d v="2025-08-28T00:00:00"/>
     <d v="2025-09-05T00:00:00"/>
@@ -3860,7 +4997,7 @@
   <r>
     <n v="43"/>
     <d v="2025-03-01T00:00:00"/>
-    <s v="Lanza C."/>
+    <x v="13"/>
     <n v="3284.5"/>
     <d v="2025-06-01T00:00:00"/>
     <d v="2025-06-20T00:00:00"/>
@@ -3871,7 +5008,7 @@
   <r>
     <n v="44"/>
     <d v="2026-01-07T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="750"/>
     <d v="2026-04-07T00:00:00"/>
     <m/>
@@ -3882,7 +5019,7 @@
   <r>
     <n v="45"/>
     <d v="2026-02-26T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="7356"/>
     <d v="2026-05-26T00:00:00"/>
     <m/>
@@ -3893,7 +5030,7 @@
   <r>
     <n v="46"/>
     <d v="2025-08-19T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="3562"/>
     <d v="2025-11-19T00:00:00"/>
     <m/>
@@ -3904,7 +5041,7 @@
   <r>
     <n v="47"/>
     <d v="2025-12-14T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="12000"/>
     <d v="2026-03-14T00:00:00"/>
     <m/>
@@ -3915,7 +5052,7 @@
   <r>
     <n v="48"/>
     <d v="2025-07-20T00:00:00"/>
-    <s v="Rossi F."/>
+    <x v="10"/>
     <n v="10200"/>
     <d v="2025-10-20T00:00:00"/>
     <d v="2025-11-01T00:00:00"/>
@@ -3926,7 +5063,7 @@
   <r>
     <n v="49"/>
     <d v="2026-02-10T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="140"/>
     <d v="2026-05-10T00:00:00"/>
     <m/>
@@ -3937,7 +5074,7 @@
   <r>
     <n v="50"/>
     <d v="2025-06-16T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="10900"/>
     <d v="2025-09-16T00:00:00"/>
     <d v="2025-09-20T00:00:00"/>
@@ -3948,7 +5085,7 @@
   <r>
     <n v="51"/>
     <d v="2025-04-28T00:00:00"/>
-    <s v="Lanza A."/>
+    <x v="6"/>
     <n v="2500"/>
     <d v="2025-07-28T00:00:00"/>
     <d v="2026-04-17T00:00:00"/>
@@ -3959,7 +5096,7 @@
   <r>
     <n v="52"/>
     <d v="2026-02-10T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="8800"/>
     <d v="2026-05-10T00:00:00"/>
     <d v="2026-01-26T00:00:00"/>
@@ -3970,7 +5107,7 @@
   <r>
     <n v="53"/>
     <d v="2024-09-12T00:00:00"/>
-    <s v="Marini E."/>
+    <x v="14"/>
     <n v="1950"/>
     <d v="2025-03-12T00:00:00"/>
     <d v="2026-03-25T00:00:00"/>
@@ -3981,7 +5118,7 @@
   <r>
     <n v="54"/>
     <d v="2025-06-04T00:00:00"/>
-    <s v="Rossi M."/>
+    <x v="0"/>
     <n v="4789.84"/>
     <d v="2025-09-04T00:00:00"/>
     <d v="2025-11-05T00:00:00"/>
@@ -3992,7 +5129,7 @@
   <r>
     <n v="55"/>
     <d v="2025-09-17T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="350"/>
     <d v="2025-12-17T00:00:00"/>
     <d v="2026-05-02T00:00:00"/>
@@ -4003,7 +5140,7 @@
   <r>
     <n v="56"/>
     <d v="2026-04-22T00:00:00"/>
-    <s v="Bianchi R."/>
+    <x v="5"/>
     <n v="1700"/>
     <d v="2026-07-22T00:00:00"/>
     <d v="2025-06-10T00:00:00"/>
@@ -4014,7 +5151,7 @@
   <r>
     <n v="57"/>
     <d v="2026-01-05T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="4600"/>
     <d v="2026-04-05T00:00:00"/>
     <d v="2025-08-28T00:00:00"/>
@@ -4025,7 +5162,7 @@
   <r>
     <n v="58"/>
     <d v="2025-10-13T00:00:00"/>
-    <s v="Lanza C."/>
+    <x v="13"/>
     <n v="550"/>
     <d v="2026-01-13T00:00:00"/>
     <d v="2025-12-20T00:00:00"/>
@@ -4036,7 +5173,7 @@
   <r>
     <n v="59"/>
     <s v="29/02/2025"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="10500"/>
     <d v="2025-05-29T00:00:00"/>
     <d v="2026-03-15T00:00:00"/>
@@ -4047,7 +5184,7 @@
   <r>
     <n v="60"/>
     <d v="2025-08-08T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="2500"/>
     <d v="2025-11-08T00:00:00"/>
     <m/>
@@ -4058,7 +5195,7 @@
   <r>
     <n v="61"/>
     <d v="2026-01-11T00:00:00"/>
-    <s v="Marini G."/>
+    <x v="15"/>
     <n v="1900"/>
     <d v="2026-04-11T00:00:00"/>
     <d v="2026-01-01T00:00:00"/>
@@ -4069,7 +5206,7 @@
   <r>
     <n v="62"/>
     <d v="2025-12-20T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="8400"/>
     <d v="2026-03-20T00:00:00"/>
     <d v="2026-07-20T00:00:00"/>
@@ -4080,7 +5217,7 @@
   <r>
     <n v="63"/>
     <d v="2025-11-07T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="3200"/>
     <d v="2026-02-07T00:00:00"/>
     <d v="2026-05-01T00:00:00"/>
@@ -4091,7 +5228,7 @@
   <r>
     <n v="64"/>
     <d v="2025-07-16T00:00:00"/>
-    <s v="Rossi F."/>
+    <x v="10"/>
     <n v="4700"/>
     <d v="2025-10-16T00:00:00"/>
     <d v="2026-03-01T00:00:00"/>
@@ -4102,7 +5239,7 @@
   <r>
     <n v="65"/>
     <d v="2026-02-02T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="1150"/>
     <d v="2026-05-02T00:00:00"/>
     <d v="2025-09-10T00:00:00"/>
@@ -4113,7 +5250,7 @@
   <r>
     <n v="66"/>
     <d v="2025-03-14T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="5300"/>
     <d v="2025-06-14T00:00:00"/>
     <d v="2025-11-15T00:00:00"/>
@@ -4124,7 +5261,7 @@
   <r>
     <n v="67"/>
     <d v="2025-05-21T00:00:00"/>
-    <s v="Bianchi A."/>
+    <x v="11"/>
     <n v="15000"/>
     <d v="2025-08-21T00:00:00"/>
     <d v="2026-03-10T00:00:00"/>
@@ -4135,7 +5272,7 @@
   <r>
     <n v="68"/>
     <d v="2025-09-10T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="650"/>
     <d v="2025-12-10T00:00:00"/>
     <d v="2026-01-15T00:00:00"/>
@@ -4146,7 +5283,7 @@
   <r>
     <n v="69"/>
     <d v="2025-10-26T00:00:00"/>
-    <s v="Lanza A."/>
+    <x v="6"/>
     <n v="2800"/>
     <d v="2026-01-26T00:00:00"/>
     <d v="2025-03-01T00:00:00"/>
@@ -4157,7 +5294,7 @@
   <r>
     <n v="70"/>
     <d v="2025-12-03T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="1850"/>
     <d v="2026-03-03T00:00:00"/>
     <d v="2025-11-10T00:00:00"/>
@@ -4168,7 +5305,7 @@
   <r>
     <n v="71"/>
     <d v="2025-04-07T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="7100"/>
     <d v="2025-09-07T00:00:00"/>
     <d v="2026-01-18T00:00:00"/>
@@ -4179,7 +5316,7 @@
   <r>
     <n v="72"/>
     <d v="2026-04-19T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="2600"/>
     <d v="2026-07-19T00:00:00"/>
     <d v="2026-03-15T00:00:00"/>
@@ -4190,7 +5327,7 @@
   <r>
     <n v="73"/>
     <d v="2025-01-01T00:00:00"/>
-    <s v="Marini E."/>
+    <x v="14"/>
     <n v="4400"/>
     <d v="2025-04-01T00:00:00"/>
     <d v="2026-02-10T00:00:00"/>
@@ -4201,7 +5338,7 @@
   <r>
     <n v="74"/>
     <d v="2025-11-11T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="9500"/>
     <d v="2026-02-11T00:00:00"/>
     <d v="2025-03-01T00:00:00"/>
@@ -4212,7 +5349,7 @@
   <r>
     <n v="75"/>
     <d v="2025-06-28T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="3300"/>
     <d v="2025-09-28T00:00:00"/>
     <d v="2025-11-20T00:00:00"/>
@@ -4223,7 +5360,7 @@
   <r>
     <n v="76"/>
     <d v="2025-08-09T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="1550"/>
     <d v="2025-11-09T00:00:00"/>
     <d v="2025-08-25T00:00:00"/>
@@ -4234,7 +5371,7 @@
   <r>
     <n v="77"/>
     <d v="2026-02-04T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="5900"/>
     <d v="2026-05-04T00:00:00"/>
     <d v="2026-05-15T00:00:00"/>
@@ -4245,7 +5382,7 @@
   <r>
     <n v="78"/>
     <d v="2025-10-18T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="2750"/>
     <d v="2026-01-18T00:00:00"/>
     <m/>
@@ -4256,7 +5393,7 @@
   <r>
     <n v="79"/>
     <d v="2024-12-01T00:00:00"/>
-    <s v="Rossi M."/>
+    <x v="0"/>
     <n v="1000"/>
     <d v="2025-03-01T00:00:00"/>
     <d v="2026-05-25T00:00:00"/>
@@ -4267,7 +5404,7 @@
   <r>
     <n v="80"/>
     <d v="2025-07-23T00:00:00"/>
-    <s v="Lanza C."/>
+    <x v="13"/>
     <n v="6800"/>
     <d v="2025-10-23T00:00:00"/>
     <d v="2026-03-20T00:00:00"/>
@@ -4278,7 +5415,7 @@
   <r>
     <n v="81"/>
     <d v="2026-04-15T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="1890.5"/>
     <d v="2026-07-15T00:00:00"/>
     <d v="2025-10-20T00:00:00"/>
@@ -4289,7 +5426,7 @@
   <r>
     <n v="82"/>
     <d v="2026-03-06T00:00:00"/>
-    <s v="Bianchi R."/>
+    <x v="5"/>
     <n v="4100"/>
     <d v="2026-03-06T00:00:00"/>
     <d v="2026-03-10T00:00:00"/>
@@ -4300,7 +5437,7 @@
   <r>
     <n v="83"/>
     <d v="2025-06-20T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="750"/>
     <d v="2025-09-20T00:00:00"/>
     <d v="2025-06-01T00:00:00"/>
@@ -4311,7 +5448,7 @@
   <r>
     <n v="84"/>
     <d v="2026-01-17T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="2980"/>
     <d v="2026-04-17T00:00:00"/>
     <d v="2025-07-01T00:00:00"/>
@@ -4322,7 +5459,7 @@
   <r>
     <n v="85"/>
     <d v="2025-08-29T00:00:00"/>
-    <s v="Marini G."/>
+    <x v="15"/>
     <n v="1250"/>
     <d v="2025-11-29T00:00:00"/>
     <d v="2025-09-01T00:00:00"/>
@@ -4333,7 +5470,7 @@
   <r>
     <n v="86"/>
     <d v="2025-09-14T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="9870.2999999999993"/>
     <d v="2025-12-14T00:00:00"/>
     <d v="2026-04-10T00:00:00"/>
@@ -4344,7 +5481,7 @@
   <r>
     <n v="87"/>
     <d v="2025-04-08T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="645"/>
     <d v="2025-07-08T00:00:00"/>
     <d v="2026-02-25T00:00:00"/>
@@ -4355,7 +5492,7 @@
   <r>
     <n v="88"/>
     <d v="2025-11-03T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="3200"/>
     <d v="2026-02-03T00:00:00"/>
     <d v="2025-06-10T00:00:00"/>
@@ -4366,7 +5503,7 @@
   <r>
     <n v="89"/>
     <d v="2025-08-24T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="150"/>
     <d v="2025-11-24T00:00:00"/>
     <d v="2026-01-01T00:00:00"/>
@@ -4377,7 +5514,7 @@
   <r>
     <n v="90"/>
     <d v="2025-02-10T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="11230"/>
     <d v="2025-05-10T00:00:00"/>
     <d v="2026-03-20T00:00:00"/>
@@ -4388,7 +5525,7 @@
   <r>
     <n v="91"/>
     <d v="2026-01-06T00:00:00"/>
-    <s v="Bianchi A."/>
+    <x v="11"/>
     <n v="4500"/>
     <d v="2026-04-06T00:00:00"/>
     <d v="2026-03-15T00:00:00"/>
@@ -4399,7 +5536,7 @@
   <r>
     <n v="92"/>
     <d v="2025-10-19T00:00:00"/>
-    <s v="Lanza A."/>
+    <x v="6"/>
     <n v="7890"/>
     <d v="2026-01-19T00:00:00"/>
     <d v="2026-02-01T00:00:00"/>
@@ -4410,7 +5547,7 @@
   <r>
     <n v="93"/>
     <d v="2025-07-01T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="1050"/>
     <d v="2025-10-01T00:00:00"/>
     <d v="2026-04-01T00:00:00"/>
@@ -4421,7 +5558,7 @@
   <r>
     <n v="94"/>
     <d v="2025-12-15T00:00:00"/>
-    <s v="Rossi F."/>
+    <x v="10"/>
     <n v="3450.9"/>
     <d v="2026-03-15T00:00:00"/>
     <d v="2026-03-15T00:00:00"/>
@@ -4432,7 +5569,7 @@
   <r>
     <n v="95"/>
     <d v="2025-05-09T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="2150"/>
     <d v="2025-08-09T00:00:00"/>
     <d v="2025-11-20T00:00:00"/>
@@ -4443,7 +5580,7 @@
   <r>
     <n v="96"/>
     <d v="2025-09-04T00:00:00"/>
-    <s v="Marini E."/>
+    <x v="14"/>
     <n v="99.5"/>
     <d v="2025-12-04T00:00:00"/>
     <d v="2026-01-20T00:00:00"/>
@@ -4454,7 +5591,7 @@
   <r>
     <n v="97"/>
     <d v="2026-04-18T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="12000"/>
     <d v="2026-07-18T00:00:00"/>
     <d v="2026-03-10T00:00:00"/>
@@ -4465,7 +5602,7 @@
   <r>
     <n v="98"/>
     <d v="2025-01-23T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="350"/>
     <d v="2025-04-23T00:00:00"/>
     <d v="2026-01-15T00:00:00"/>
@@ -4476,7 +5613,7 @@
   <r>
     <n v="99"/>
     <d v="2025-12-07T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="6700"/>
     <d v="2026-03-07T00:00:00"/>
     <d v="2025-06-01T00:00:00"/>
@@ -4487,7 +5624,7 @@
   <r>
     <n v="100"/>
     <d v="2026-02-21T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="1450"/>
     <d v="2026-05-21T00:00:00"/>
     <d v="2025-09-01T00:00:00"/>
@@ -4498,7 +5635,7 @@
   <r>
     <n v="101"/>
     <d v="2025-07-05T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="8200"/>
     <d v="2025-10-05T00:00:00"/>
     <d v="2025-09-20T00:00:00"/>
@@ -4509,7 +5646,7 @@
   <r>
     <n v="102"/>
     <d v="2025-08-29T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="500"/>
     <d v="2025-11-29T00:00:00"/>
     <d v="2026-04-15T00:00:00"/>
@@ -4520,7 +5657,7 @@
   <r>
     <n v="103"/>
     <d v="2026-01-11T00:00:00"/>
-    <s v="Lanza C."/>
+    <x v="13"/>
     <n v="3750"/>
     <d v="2026-04-11T00:00:00"/>
     <m/>
@@ -4531,7 +5668,7 @@
   <r>
     <n v="104"/>
     <d v="2025-12-14T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="2900"/>
     <d v="2026-03-14T00:00:00"/>
     <d v="2025-09-24T00:00:00"/>
@@ -4542,7 +5679,7 @@
   <r>
     <n v="105"/>
     <d v="2026-02-03T00:00:00"/>
-    <s v="Rossi M."/>
+    <x v="0"/>
     <n v="1600"/>
     <d v="2026-05-03T00:00:00"/>
     <m/>
@@ -4553,7 +5690,7 @@
   <r>
     <n v="106"/>
     <d v="2025-06-16T00:00:00"/>
-    <s v="Bianchi R."/>
+    <x v="5"/>
     <n v="450"/>
     <d v="2025-09-16T00:00:00"/>
     <d v="2026-03-10T00:00:00"/>
@@ -4564,7 +5701,7 @@
   <r>
     <n v="107"/>
     <d v="2025-10-01T00:00:00"/>
-    <s v="Marini G."/>
+    <x v="15"/>
     <n v="1830"/>
     <d v="2026-01-01T00:00:00"/>
     <m/>
@@ -4575,7 +5712,7 @@
   <r>
     <n v="108"/>
     <d v="2025-02-27T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="9000"/>
     <d v="2025-05-27T00:00:00"/>
     <d v="2026-05-10T00:00:00"/>
@@ -4586,7 +5723,7 @@
   <r>
     <n v="109"/>
     <d v="2025-11-19T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="125"/>
     <d v="2026-02-19T00:00:00"/>
     <d v="2025-09-01T00:00:00"/>
@@ -4597,7 +5734,7 @@
   <r>
     <n v="110"/>
     <d v="2025-09-12T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="5100"/>
     <d v="2025-12-12T00:00:00"/>
     <d v="2025-08-20T00:00:00"/>
@@ -4608,7 +5745,7 @@
   <r>
     <n v="111"/>
     <d v="2025-01-08T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="1100"/>
     <d v="2025-04-08T00:00:00"/>
     <d v="2026-05-20T00:00:00"/>
@@ -4619,7 +5756,7 @@
   <r>
     <n v="112"/>
     <d v="2025-06-04T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="15000"/>
     <d v="2025-09-04T00:00:00"/>
     <m/>
@@ -4630,7 +5767,7 @@
   <r>
     <n v="113"/>
     <d v="2026-04-21T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="2340"/>
     <d v="2026-07-21T00:00:00"/>
     <m/>
@@ -4641,7 +5778,7 @@
   <r>
     <n v="114"/>
     <d v="2026-03-15T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="7900"/>
     <d v="2026-06-15T00:00:00"/>
     <d v="2025-12-20T00:00:00"/>
@@ -4652,7 +5789,7 @@
   <r>
     <n v="115"/>
     <d v="2025-08-03T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="400"/>
     <d v="2025-11-03T00:00:00"/>
     <d v="2026-04-15T00:00:00"/>
@@ -4663,7 +5800,7 @@
   <r>
     <n v="116"/>
     <d v="2025-12-28T00:00:00"/>
-    <s v="Lanza A."/>
+    <x v="6"/>
     <n v="1700"/>
     <d v="2026-03-28T00:00:00"/>
     <d v="2025-06-01T00:00:00"/>
@@ -4674,7 +5811,7 @@
   <r>
     <n v="117"/>
     <d v="2025-10-09T00:00:00"/>
-    <s v="Rossi F."/>
+    <x v="10"/>
     <n v="5600"/>
     <d v="2026-01-09T00:00:00"/>
     <m/>
@@ -4685,7 +5822,7 @@
   <r>
     <n v="118"/>
     <d v="2026-02-20T00:00:00"/>
-    <s v="Bianchi A."/>
+    <x v="11"/>
     <n v="9200"/>
     <d v="2026-05-20T00:00:00"/>
     <d v="2025-11-15T00:00:00"/>
@@ -4696,7 +5833,7 @@
   <r>
     <n v="119"/>
     <d v="2025-04-01T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="3100"/>
     <d v="2025-07-01T00:00:00"/>
     <d v="2026-03-20T00:00:00"/>
@@ -4707,7 +5844,7 @@
   <r>
     <n v="120"/>
     <d v="2026-01-14T00:00:00"/>
-    <s v="Marini E."/>
+    <x v="14"/>
     <n v="1200"/>
     <d v="2026-04-14T00:00:00"/>
     <d v="2025-07-01T00:00:00"/>
@@ -4718,7 +5855,7 @@
   <r>
     <n v="121"/>
     <d v="2025-11-26T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="800"/>
     <d v="2026-02-26T00:00:00"/>
     <d v="2025-11-20T00:00:00"/>
@@ -4729,7 +5866,7 @@
   <r>
     <n v="122"/>
     <d v="2025-09-10T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="5500"/>
     <d v="2025-12-10T00:00:00"/>
     <m/>
@@ -4740,7 +5877,7 @@
   <r>
     <n v="123"/>
     <d v="2026-01-05T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="12500"/>
     <d v="2026-04-05T00:00:00"/>
     <d v="2026-05-20T00:00:00"/>
@@ -4751,7 +5888,7 @@
   <r>
     <n v="124"/>
     <d v="2025-08-23T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="4800"/>
     <d v="2025-11-23T00:00:00"/>
     <d v="2025-08-01T00:00:00"/>
@@ -4762,7 +5899,7 @@
   <r>
     <n v="125"/>
     <d v="2025-12-17T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="1950"/>
     <d v="2026-03-17T00:00:00"/>
     <m/>
@@ -4773,7 +5910,7 @@
   <r>
     <n v="126"/>
     <d v="2025-06-19T00:00:00"/>
-    <s v="Lanza C."/>
+    <x v="13"/>
     <n v="6000"/>
     <d v="2025-09-19T00:00:00"/>
     <d v="2025-12-10T00:00:00"/>
@@ -4784,7 +5921,7 @@
   <r>
     <n v="127"/>
     <d v="2024-12-08T00:00:00"/>
-    <s v="Rossi M."/>
+    <x v="0"/>
     <n v="300"/>
     <d v="2025-03-08T00:00:00"/>
     <d v="2026-02-15T00:00:00"/>
@@ -4795,7 +5932,7 @@
   <r>
     <n v="128"/>
     <d v="2025-11-02T00:00:00"/>
-    <s v="Bianchi R."/>
+    <x v="5"/>
     <n v="250"/>
     <d v="2026-02-02T00:00:00"/>
     <d v="2026-03-10T00:00:00"/>
@@ -4806,7 +5943,7 @@
   <r>
     <n v="129"/>
     <d v="2026-01-20T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="8800"/>
     <d v="2026-04-20T00:00:00"/>
     <d v="2026-07-20T00:00:00"/>
@@ -4817,7 +5954,7 @@
   <r>
     <n v="130"/>
     <d v="2025-04-06T00:00:00"/>
-    <s v="Marini G."/>
+    <x v="15"/>
     <n v="1100"/>
     <d v="2025-07-06T00:00:00"/>
     <d v="2026-04-20T00:00:00"/>
@@ -4828,7 +5965,7 @@
   <r>
     <n v="131"/>
     <d v="2026-02-13T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="4300"/>
     <d v="2026-05-13T00:00:00"/>
     <d v="2026-05-15T00:00:00"/>
@@ -4839,7 +5976,7 @@
   <r>
     <n v="132"/>
     <d v="2025-10-18T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="900"/>
     <d v="2026-01-18T00:00:00"/>
     <d v="2026-03-10T00:00:00"/>
@@ -4850,7 +5987,7 @@
   <r>
     <n v="133"/>
     <d v="2025-07-24T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="1750"/>
     <d v="2025-10-24T00:00:00"/>
     <d v="2025-06-01T00:00:00"/>
@@ -4861,7 +5998,7 @@
   <r>
     <n v="134"/>
     <d v="2026-01-07T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="2900"/>
     <d v="2026-04-07T00:00:00"/>
     <d v="2026-01-15T00:00:00"/>
@@ -4872,7 +6009,7 @@
   <r>
     <n v="135"/>
     <d v="2025-12-29T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="6200"/>
     <d v="2026-03-29T00:00:00"/>
     <d v="2025-11-10T00:00:00"/>
@@ -4883,7 +6020,7 @@
   <r>
     <n v="136"/>
     <d v="2025-08-10T00:00:00"/>
-    <s v="Lanza A."/>
+    <x v="6"/>
     <n v="3600"/>
     <d v="2025-11-10T00:00:00"/>
     <d v="2026-03-10T00:00:00"/>
@@ -4894,7 +6031,7 @@
   <r>
     <n v="137"/>
     <d v="2026-02-04T00:00:00"/>
-    <s v="Rossi F."/>
+    <x v="10"/>
     <n v="1500"/>
     <d v="2026-05-04T00:00:00"/>
     <d v="2026-05-10T00:00:00"/>
@@ -4905,7 +6042,7 @@
   <r>
     <n v="138"/>
     <d v="2025-09-12T00:00:00"/>
-    <s v="Bianchi A."/>
+    <x v="11"/>
     <n v="4900"/>
     <d v="2026-03-12T00:00:00"/>
     <d v="2025-11-20T00:00:00"/>
@@ -4916,7 +6053,7 @@
   <r>
     <n v="139"/>
     <d v="2025-03-01T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="2100"/>
     <d v="2025-06-01T00:00:00"/>
     <d v="2026-01-10T00:00:00"/>
@@ -4927,7 +6064,7 @@
   <r>
     <n v="140"/>
     <d v="2025-08-17T00:00:00"/>
-    <s v="Marini E."/>
+    <x v="14"/>
     <n v="7300"/>
     <d v="2025-11-17T00:00:00"/>
     <d v="2026-03-15T00:00:00"/>
@@ -4938,7 +6075,7 @@
   <r>
     <n v="141"/>
     <d v="2025-05-21T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="180"/>
     <d v="2025-08-21T00:00:00"/>
     <d v="2025-07-01T00:00:00"/>
@@ -4949,7 +6086,7 @@
   <r>
     <n v="142"/>
     <d v="2025-10-15T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="5400"/>
     <d v="2026-01-15T00:00:00"/>
     <d v="2026-03-15T00:00:00"/>
@@ -4960,7 +6097,7 @@
   <r>
     <n v="143"/>
     <d v="2026-04-28T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="1350"/>
     <d v="2026-07-28T00:00:00"/>
     <m/>
@@ -4971,7 +6108,7 @@
   <r>
     <n v="144"/>
     <d v="2025-02-03T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="9800"/>
     <d v="2025-05-03T00:00:00"/>
     <d v="2026-05-20T00:00:00"/>
@@ -4982,7 +6119,7 @@
   <r>
     <n v="145"/>
     <d v="2025-07-16T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="450"/>
     <d v="2025-10-16T00:00:00"/>
     <d v="2026-05-20T00:00:00"/>
@@ -4993,7 +6130,7 @@
   <r>
     <n v="146"/>
     <d v="2025-11-08T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="2700"/>
     <d v="2026-02-08T00:00:00"/>
     <d v="2026-05-01T00:00:00"/>
@@ -5004,7 +6141,7 @@
   <r>
     <n v="147"/>
     <d v="2025-09-23T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="6500"/>
     <d v="2025-12-23T00:00:00"/>
     <d v="2026-03-15T00:00:00"/>
@@ -5015,7 +6152,7 @@
   <r>
     <n v="148"/>
     <d v="2025-12-11T00:00:00"/>
-    <s v="Lanza C."/>
+    <x v="13"/>
     <n v="3900"/>
     <d v="2026-03-11T00:00:00"/>
     <d v="2025-11-20T00:00:00"/>
@@ -5026,7 +6163,7 @@
   <r>
     <n v="149"/>
     <d v="2026-04-20T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="8100"/>
     <d v="2026-07-20T00:00:00"/>
     <d v="2026-03-15T00:00:00"/>
@@ -5037,7 +6174,7 @@
   <r>
     <n v="150"/>
     <d v="2025-06-05T00:00:00"/>
-    <s v="Rossi M."/>
+    <x v="0"/>
     <n v="12000"/>
     <d v="2025-09-05T00:00:00"/>
     <d v="2025-09-20T00:00:00"/>
@@ -5048,7 +6185,7 @@
   <r>
     <n v="151"/>
     <d v="2026-01-17T00:00:00"/>
-    <s v="Bianchi R."/>
+    <x v="5"/>
     <n v="2200"/>
     <d v="2026-04-17T00:00:00"/>
     <d v="2025-05-01T00:00:00"/>
@@ -5059,7 +6196,7 @@
   <r>
     <n v="152"/>
     <d v="2026-02-12T00:00:00"/>
-    <s v="Marini G."/>
+    <x v="15"/>
     <n v="1400"/>
     <d v="2026-05-12T00:00:00"/>
     <d v="2026-03-10T00:00:00"/>
@@ -5070,7 +6207,7 @@
   <r>
     <n v="153"/>
     <d v="2025-05-25T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="7700"/>
     <d v="2025-08-25T00:00:00"/>
     <d v="2025-05-20T00:00:00"/>
@@ -5081,7 +6218,7 @@
   <r>
     <n v="154"/>
     <d v="2025-12-10T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="3500"/>
     <d v="2026-03-10T00:00:00"/>
     <d v="2025-09-20T00:00:00"/>
@@ -5092,7 +6229,7 @@
   <r>
     <n v="155"/>
     <d v="2025-02-01T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="9000"/>
     <d v="2025-05-01T00:00:00"/>
     <m/>
@@ -5103,7 +6240,7 @@
   <r>
     <n v="156"/>
     <d v="2025-06-15T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="1600"/>
     <d v="2025-09-15T00:00:00"/>
     <m/>
@@ -5114,7 +6251,7 @@
   <r>
     <n v="157"/>
     <d v="2025-08-05T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="4600"/>
     <d v="2025-11-05T00:00:00"/>
     <d v="2025-04-25T00:00:00"/>
@@ -5125,7 +6262,7 @@
   <r>
     <n v="158"/>
     <d v="2026-04-20T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="550"/>
     <d v="2026-07-20T00:00:00"/>
     <d v="2026-01-25T00:00:00"/>
@@ -5136,7 +6273,7 @@
   <r>
     <n v="159"/>
     <d v="2025-01-11T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="10500"/>
     <d v="2025-04-11T00:00:00"/>
     <d v="2025-03-20T00:00:00"/>
@@ -5147,7 +6284,7 @@
   <r>
     <n v="160"/>
     <d v="2025-10-03T00:00:00"/>
-    <s v="Lanza A."/>
+    <x v="6"/>
     <n v="2500"/>
     <d v="2026-01-03T00:00:00"/>
     <m/>
@@ -5158,7 +6295,7 @@
   <r>
     <n v="161"/>
     <d v="2024-12-18T00:00:00"/>
-    <s v="Rossi F."/>
+    <x v="10"/>
     <n v="1900"/>
     <d v="2025-03-18T00:00:00"/>
     <d v="2025-05-05T00:00:00"/>
@@ -5169,7 +6306,7 @@
   <r>
     <n v="162"/>
     <d v="2025-11-02T00:00:00"/>
-    <s v="Bianchi A."/>
+    <x v="11"/>
     <n v="8400"/>
     <d v="2026-02-02T00:00:00"/>
     <m/>
@@ -5180,7 +6317,7 @@
   <r>
     <n v="163"/>
     <d v="2025-01-29T00:00:00"/>
-    <s v="Marini E."/>
+    <x v="14"/>
     <n v="3200"/>
     <d v="2025-04-29T00:00:00"/>
     <d v="2025-08-01T00:00:00"/>
@@ -5191,7 +6328,7 @@
   <r>
     <n v="164"/>
     <d v="2025-09-14T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="4700"/>
     <d v="2025-12-14T00:00:00"/>
     <m/>
@@ -5202,7 +6339,7 @@
   <r>
     <n v="165"/>
     <d v="2025-04-08T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="1150"/>
     <d v="2025-07-08T00:00:00"/>
     <m/>
@@ -5213,7 +6350,7 @@
   <r>
     <n v="166"/>
     <d v="2025-10-22T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="5300"/>
     <d v="2026-01-22T00:00:00"/>
     <d v="2025-06-15T00:00:00"/>
@@ -5224,7 +6361,7 @@
   <r>
     <n v="167"/>
     <d v="2026-01-17T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="15000"/>
     <d v="2026-04-17T00:00:00"/>
     <m/>
@@ -5235,7 +6372,7 @@
   <r>
     <n v="168"/>
     <d v="2025-03-06T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="650"/>
     <d v="2025-06-06T00:00:00"/>
     <m/>
@@ -5246,7 +6383,7 @@
   <r>
     <n v="169"/>
     <d v="2025-12-09T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="2800"/>
     <d v="2026-03-09T00:00:00"/>
     <d v="2025-04-20T00:00:00"/>
@@ -5257,7 +6394,7 @@
   <r>
     <n v="170"/>
     <d v="2025-11-19T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="1850"/>
     <d v="2026-02-19T00:00:00"/>
     <d v="2025-11-01T00:00:00"/>
@@ -5268,7 +6405,7 @@
   <r>
     <n v="171"/>
     <d v="2025-01-21T00:00:00"/>
-    <s v="Lanza C."/>
+    <x v="13"/>
     <n v="7100"/>
     <d v="2025-04-21T00:00:00"/>
     <m/>
@@ -5279,7 +6416,7 @@
   <r>
     <n v="172"/>
     <d v="2025-07-04T00:00:00"/>
-    <s v="Rossi M."/>
+    <x v="0"/>
     <n v="2600"/>
     <d v="2025-10-04T00:00:00"/>
     <d v="2026-01-01T00:00:00"/>
@@ -5290,7 +6427,7 @@
   <r>
     <n v="173"/>
     <d v="2025-12-07T00:00:00"/>
-    <s v="Bianchi R."/>
+    <x v="5"/>
     <n v="4400"/>
     <d v="2026-03-07T00:00:00"/>
     <m/>
@@ -5301,7 +6438,7 @@
   <r>
     <n v="174"/>
     <d v="2025-09-23T00:00:00"/>
-    <s v="Marini G."/>
+    <x v="15"/>
     <n v="9500"/>
     <d v="2025-12-23T00:00:00"/>
     <d v="2025-07-15T00:00:00"/>
@@ -5312,7 +6449,7 @@
   <r>
     <n v="175"/>
     <d v="2026-02-13T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="3300"/>
     <d v="2026-05-13T00:00:00"/>
     <m/>
@@ -5323,7 +6460,7 @@
   <r>
     <n v="176"/>
     <d v="2025-04-01T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="1550"/>
     <d v="2025-07-01T00:00:00"/>
     <d v="2025-06-05T00:00:00"/>
@@ -5334,7 +6471,7 @@
   <r>
     <n v="177"/>
     <d v="2025-12-17T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="5900"/>
     <d v="2026-03-17T00:00:00"/>
     <d v="2025-11-10T00:00:00"/>
@@ -5345,7 +6482,7 @@
   <r>
     <n v="178"/>
     <d v="2025-02-28T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="2750"/>
     <d v="2025-05-28T00:00:00"/>
     <m/>
@@ -5356,7 +6493,7 @@
   <r>
     <n v="179"/>
     <d v="2025-08-02T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="1000"/>
     <d v="2025-11-02T00:00:00"/>
     <d v="2025-04-20T00:00:00"/>
@@ -5367,7 +6504,7 @@
   <r>
     <n v="180"/>
     <d v="2025-10-11T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="6800"/>
     <d v="2026-01-11T00:00:00"/>
     <d v="2025-06-10T00:00:00"/>
@@ -5378,7 +6515,7 @@
   <r>
     <n v="181"/>
     <d v="2025-01-04T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="1890.5"/>
     <d v="2025-04-04T00:00:00"/>
     <m/>
@@ -5389,7 +6526,7 @@
   <r>
     <n v="182"/>
     <d v="2025-03-16T00:00:00"/>
-    <s v="Lanza A."/>
+    <x v="6"/>
     <n v="4100"/>
     <d v="2025-06-16T00:00:00"/>
     <m/>
@@ -5400,7 +6537,7 @@
   <r>
     <n v="183"/>
     <d v="2025-11-27T00:00:00"/>
-    <s v="Pinca V."/>
+    <x v="8"/>
     <n v="750"/>
     <d v="2026-02-27T00:00:00"/>
     <d v="2025-10-01T00:00:00"/>
@@ -5411,7 +6548,7 @@
   <r>
     <n v="184"/>
     <d v="2026-01-12T00:00:00"/>
-    <s v="Rossi F."/>
+    <x v="10"/>
     <n v="2980"/>
     <d v="2026-04-12T00:00:00"/>
     <d v="2025-03-20T00:00:00"/>
@@ -5422,7 +6559,7 @@
   <r>
     <n v="185"/>
     <d v="2025-06-05T00:00:00"/>
-    <s v="Bianchi A."/>
+    <x v="11"/>
     <n v="1250"/>
     <d v="2025-09-05T00:00:00"/>
     <d v="2025-11-15T00:00:00"/>
@@ -5433,7 +6570,7 @@
   <r>
     <n v="186"/>
     <d v="2024-12-20T00:00:00"/>
-    <s v="Marini E."/>
+    <x v="14"/>
     <n v="9870.2999999999993"/>
     <d v="2025-03-20T00:00:00"/>
     <d v="2025-09-15T00:00:00"/>
@@ -5444,7 +6581,7 @@
   <r>
     <n v="187"/>
     <d v="2025-08-13T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="645"/>
     <d v="2025-11-13T00:00:00"/>
     <d v="2025-11-01T00:00:00"/>
@@ -5455,7 +6592,7 @@
   <r>
     <n v="188"/>
     <d v="2025-05-09T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="3200"/>
     <d v="2025-08-09T00:00:00"/>
     <m/>
@@ -5466,7 +6603,7 @@
   <r>
     <n v="189"/>
     <d v="2025-07-24T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="150"/>
     <d v="2025-10-24T00:00:00"/>
     <d v="2025-03-20T00:00:00"/>
@@ -5477,7 +6614,7 @@
   <r>
     <n v="190"/>
     <d v="2026-02-03T00:00:00"/>
-    <s v="Villani"/>
+    <x v="4"/>
     <n v="11230"/>
     <d v="2026-05-03T00:00:00"/>
     <m/>
@@ -5488,7 +6625,7 @@
   <r>
     <n v="191"/>
     <d v="2024-12-15T00:00:00"/>
-    <s v="Fornari"/>
+    <x v="12"/>
     <n v="4500"/>
     <d v="2025-03-15T00:00:00"/>
     <d v="2025-12-15T00:00:00"/>
@@ -5499,7 +6636,7 @@
   <r>
     <n v="192"/>
     <d v="2025-10-21T00:00:00"/>
-    <s v="Trefoloni"/>
+    <x v="7"/>
     <n v="7890"/>
     <d v="2026-01-21T00:00:00"/>
     <d v="2025-09-05T00:00:00"/>
@@ -5510,7 +6647,7 @@
   <r>
     <n v="193"/>
     <d v="2025-09-10T00:00:00"/>
-    <s v="Lanza C."/>
+    <x v="13"/>
     <n v="1050"/>
     <d v="2025-12-10T00:00:00"/>
     <d v="2025-06-20T00:00:00"/>
@@ -5521,7 +6658,7 @@
   <r>
     <n v="194"/>
     <d v="2025-05-28T00:00:00"/>
-    <s v="Rossi M."/>
+    <x v="0"/>
     <n v="3450.9"/>
     <d v="2025-08-28T00:00:00"/>
     <m/>
@@ -5532,7 +6669,7 @@
   <r>
     <n v="195"/>
     <d v="2025-03-01T00:00:00"/>
-    <s v="Bianchi R."/>
+    <x v="5"/>
     <n v="2150"/>
     <d v="2025-06-01T00:00:00"/>
     <m/>
@@ -5543,7 +6680,7 @@
   <r>
     <n v="196"/>
     <d v="2026-01-07T00:00:00"/>
-    <s v="Marini G."/>
+    <x v="15"/>
     <n v="99.5"/>
     <d v="2026-04-07T00:00:00"/>
     <m/>
@@ -5554,7 +6691,7 @@
   <r>
     <n v="197"/>
     <d v="2026-02-26T00:00:00"/>
-    <s v="Pinca S."/>
+    <x v="1"/>
     <n v="12000"/>
     <d v="2026-05-26T00:00:00"/>
     <m/>
@@ -5565,7 +6702,7 @@
   <r>
     <n v="198"/>
     <d v="2025-11-19T00:00:00"/>
-    <s v="Sereni"/>
+    <x v="2"/>
     <n v="350"/>
     <d v="2026-02-19T00:00:00"/>
     <d v="2025-11-01T00:00:00"/>
@@ -5576,7 +6713,7 @@
   <r>
     <n v="199"/>
     <d v="2025-12-14T00:00:00"/>
-    <s v="Scottà"/>
+    <x v="3"/>
     <n v="6700"/>
     <d v="2026-03-14T00:00:00"/>
     <m/>
@@ -5587,7 +6724,7 @@
   <r>
     <n v="200"/>
     <d v="2025-07-20T00:00:00"/>
-    <s v="Risti"/>
+    <x v="9"/>
     <n v="1450"/>
     <d v="2025-10-20T00:00:00"/>
     <d v="2025-09-20T00:00:00"/>
@@ -5599,7 +6736,144 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9AF67EA-B7F4-48A0-B9DF-28596B9CC96C}" name="Tabella pivot2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13" rowHeaderCaption="Calculated Status">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{460FA36B-3688-419E-8215-F77B84CB7563}" name="Tabella pivot3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total Amount" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Customer">
+  <location ref="Z1:AA18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="9">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="17">
+        <item x="11"/>
+        <item x="5"/>
+        <item x="12"/>
+        <item x="6"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="17">
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Invoice Total" fld="3" baseField="2" baseItem="9" numFmtId="164"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9AF67EA-B7F4-48A0-B9DF-28596B9CC96C}" name="Tabella pivot2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13" rowHeaderCaption="Calculated Status">
   <location ref="M1:N5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -5701,8 +6975,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{196B16F7-4DED-4405-8DBA-D4AF07510499}" name="Tabella pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Calculated Status">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{196B16F7-4DED-4405-8DBA-D4AF07510499}" name="Tabella pivot1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Calculated Status">
   <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0"/>
@@ -10036,9 +11310,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD82BC1-84A4-4280-BEAB-AE99592285DD}">
   <dimension ref="A1:I201"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D152" sqref="D152"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F193" sqref="F193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16193,7 +17467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A164D69F-5719-4ECE-A976-CD9A45525F6C}">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -16946,10 +18220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D593E3-7876-49B2-AB89-4C24A8E228CA}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:AA18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AR22" sqref="AR22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16958,9 +18232,11 @@
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>23</v>
       </c>
@@ -16973,8 +18249,14 @@
       <c r="N1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="Z1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -16987,8 +18269,14 @@
       <c r="N2" s="23">
         <v>59063.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="Z2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="26">
+        <v>87093.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -17001,8 +18289,14 @@
       <c r="N3" s="23">
         <v>601412.84000000008</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="Z3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="26">
+        <v>84414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -17015,8 +18309,14 @@
       <c r="N4" s="23">
         <v>164252.51</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="Z4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="26">
+        <v>76889.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -17029,9 +18329,119 @@
       <c r="N5" s="23">
         <v>824728.75000000012</v>
       </c>
+      <c r="Z5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA5" s="26">
+        <v>63524</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA6" s="26">
+        <v>62450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA7" s="26">
+        <v>61494.36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="26">
+        <v>55903.979999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA9" s="26">
+        <v>51475.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA10" s="26">
+        <v>48792.619999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA11" s="26">
+        <v>48190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA12" s="26">
+        <v>44341.479999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA13" s="26">
+        <v>37947.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA14" s="26">
+        <v>33615.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA15" s="26">
+        <v>28290.74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA16" s="26">
+        <v>23166.67</v>
+      </c>
+    </row>
+    <row r="17" spans="26:27" x14ac:dyDescent="0.35">
+      <c r="Z17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA17" s="26">
+        <v>17139.5</v>
+      </c>
+    </row>
+    <row r="18" spans="26:27" x14ac:dyDescent="0.35">
+      <c r="Z18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA18" s="26">
+        <v>824728.75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Finalize Advanced Risk Analysis and Complete Project Documentation
This commit finalizes the advanced credit risk analysis sections and completes all project documentation in the README.md.

Key features and documentation:

* **Customer Concentration Risk (Section 9):** Implemented and formatted Pivot Table 3 and the Horizontal Bar Chart ("Customer Revenue Ranking"). Ensured correct ranking order for visual assessment of client dependency.
* **Late Payment Trend Analysis (Section 10):** Created and finalized the Scatter Plot ("Late Payment Trend Analysis"), filtered to analyze only overdue invoices. The analysis concludes there is **no significant linear correlation** between invoice value and payment delay.
* **Documentation Completion:** Updated and finalized Sections 9 and 10 in the README.md, including analytical conclusions and references for all required screenshots (screenshot_10, screenshot_11, and screenshot_12).
</commit_message>
<xml_diff>
--- a/Customer_Invoice_Analysis - filled.xlsx
+++ b/Customer_Invoice_Analysis - filled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\invoice-analysis-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C7B82D-312E-45A9-A5F2-858FD1880813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C56B1-7108-4AC9-A758-5997A6EFBC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{56643878-06B9-462D-81B7-435828026F01}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{56643878-06B9-462D-81B7-435828026F01}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice_Master_Data" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,12 @@
     <sheet name="Dashboard" sheetId="3" r:id="rId3"/>
     <sheet name="Reporting" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Analysis_Sheet!$I$1:$I$201</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -402,13 +405,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Colore 3" xfId="5" builtinId="39"/>
@@ -2256,7 +2259,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2716,6 +2719,1651 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Late Payment Trend Analysis</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Analysis_Sheet!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Days Overdue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Analysis_Sheet!$D$2:$D$201</c:f>
+              <c:numCache>
+                <c:formatCode>_-"€"* #,##0.00_-;\-"€"* #,##0.00_-;_-"€"* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="200"/>
+                <c:pt idx="0">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3562</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>399.36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7916.67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3360</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1839.36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>477.48</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3284.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4320</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9600</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2112.6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>534</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8600</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20112.62</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23456</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1560</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9600</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4259.9399999999996</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6780</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>477.48</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3284.5</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7356</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3562</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10200</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>10900</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4789.84</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>8400</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5300</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7100</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1550</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1890.5</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2980</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>9870.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>11230</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>7890</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3450.9</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2150</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>99.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6700</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>8200</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1830</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>5100</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>2340</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>7900</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>5600</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>9200</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>4900</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>7300</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>9800</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>8100</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>7700</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>8400</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>4700</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>5300</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>7100</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>1550</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>5900</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>2750</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1890.5</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>4100</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>2980</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>9870.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>645</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>11230</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>7890</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>3450.9</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>2150</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>99.5</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>6700</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>1450</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Analysis_Sheet!$I$2:$I$201</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="200"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-49F3-45A9-BF95-34BC12E60D16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="126209343"/>
+        <c:axId val="126204543"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="126209343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t>Invoice Amount (€)</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT" sz="1600" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.39607788828095419"/>
+              <c:y val="0.92727840335786493"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-1800000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="126204543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="126204543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t>Days Overdue</a:t>
+                </a:r>
+                <a:endParaRPr lang="it-IT" sz="1600" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.0059878721693059E-2"/>
+              <c:y val="0.34840845742629062"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="126209343"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2797,6 +4445,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4354,6 +6042,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4459,6 +6663,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>589642</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>172357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>263072</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>54427</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Grafico 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B22F26A9-9AA1-4C0B-A6E0-E5A3806DDF2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6736,7 +8978,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{460FA36B-3688-419E-8215-F77B84CB7563}" name="Tabella pivot3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total Amount" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Customer">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{460FA36B-3688-419E-8215-F77B84CB7563}" name="Tabella pivot3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total Amount" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" rowHeaderCaption="Customer">
   <location ref="Z1:AA18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -6873,7 +9115,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9AF67EA-B7F4-48A0-B9DF-28596B9CC96C}" name="Tabella pivot2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13" rowHeaderCaption="Calculated Status">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9AF67EA-B7F4-48A0-B9DF-28596B9CC96C}" name="Tabella pivot2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="13" rowHeaderCaption="Calculated Status">
   <location ref="M1:N5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -6976,7 +9218,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{196B16F7-4DED-4405-8DBA-D4AF07510499}" name="Tabella pivot1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Calculated Status">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{196B16F7-4DED-4405-8DBA-D4AF07510499}" name="Tabella pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" grandTotalCaption="Total" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7" rowHeaderCaption="Calculated Status">
   <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0"/>
@@ -11312,7 +13554,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F193" sqref="F193"/>
+      <selection pane="bottomLeft" activeCell="F205" sqref="F205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17448,6 +19690,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="I1:I201" xr:uid="{ADD82BC1-84A4-4280-BEAB-AE99592285DD}"/>
   <conditionalFormatting sqref="H1:H1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Unpaid"</formula>
@@ -17467,8 +19710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A164D69F-5719-4ECE-A976-CD9A45525F6C}">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17490,14 +19733,14 @@
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="G2" s="24" t="s">
+      <c r="D2" s="26"/>
+      <c r="G2" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -17567,14 +19810,14 @@
       <c r="A9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="G9" s="24" t="s">
+      <c r="D9" s="26"/>
+      <c r="G9" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="25"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
@@ -18222,8 +20465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D593E3-7876-49B2-AB89-4C24A8E228CA}">
   <dimension ref="A1:AA18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AR22" sqref="AR22"/>
+    <sheetView topLeftCell="AL7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18233,7 +20476,7 @@
     <col min="13" max="13" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
@@ -18272,7 +20515,7 @@
       <c r="Z2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="26">
+      <c r="AA2" s="24">
         <v>87093.3</v>
       </c>
     </row>
@@ -18292,7 +20535,7 @@
       <c r="Z3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="AA3" s="26">
+      <c r="AA3" s="24">
         <v>84414</v>
       </c>
     </row>
@@ -18312,7 +20555,7 @@
       <c r="Z4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AA4" s="26">
+      <c r="AA4" s="24">
         <v>76889.8</v>
       </c>
     </row>
@@ -18332,7 +20575,7 @@
       <c r="Z5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AA5" s="26">
+      <c r="AA5" s="24">
         <v>63524</v>
       </c>
     </row>
@@ -18340,7 +20583,7 @@
       <c r="Z6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AA6" s="26">
+      <c r="AA6" s="24">
         <v>62450</v>
       </c>
     </row>
@@ -18348,7 +20591,7 @@
       <c r="Z7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="AA7" s="26">
+      <c r="AA7" s="24">
         <v>61494.36</v>
       </c>
     </row>
@@ -18356,7 +20599,7 @@
       <c r="Z8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="AA8" s="26">
+      <c r="AA8" s="24">
         <v>55903.979999999996</v>
       </c>
     </row>
@@ -18364,7 +20607,7 @@
       <c r="Z9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="AA9" s="26">
+      <c r="AA9" s="24">
         <v>51475.8</v>
       </c>
     </row>
@@ -18372,7 +20615,7 @@
       <c r="Z10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AA10" s="26">
+      <c r="AA10" s="24">
         <v>48792.619999999995</v>
       </c>
     </row>
@@ -18380,7 +20623,7 @@
       <c r="Z11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AA11" s="26">
+      <c r="AA11" s="24">
         <v>48190</v>
       </c>
     </row>
@@ -18388,7 +20631,7 @@
       <c r="Z12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AA12" s="26">
+      <c r="AA12" s="24">
         <v>44341.479999999996</v>
       </c>
     </row>
@@ -18396,7 +20639,7 @@
       <c r="Z13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AA13" s="26">
+      <c r="AA13" s="24">
         <v>37947.1</v>
       </c>
     </row>
@@ -18404,7 +20647,7 @@
       <c r="Z14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AA14" s="26">
+      <c r="AA14" s="24">
         <v>33615.4</v>
       </c>
     </row>
@@ -18412,7 +20655,7 @@
       <c r="Z15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="AA15" s="26">
+      <c r="AA15" s="24">
         <v>28290.74</v>
       </c>
     </row>
@@ -18420,7 +20663,7 @@
       <c r="Z16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AA16" s="26">
+      <c r="AA16" s="24">
         <v>23166.67</v>
       </c>
     </row>
@@ -18428,7 +20671,7 @@
       <c r="Z17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="AA17" s="26">
+      <c r="AA17" s="24">
         <v>17139.5</v>
       </c>
     </row>
@@ -18436,7 +20679,7 @@
       <c r="Z18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AA18" s="26">
+      <c r="AA18" s="24">
         <v>824728.75</v>
       </c>
     </row>

</xml_diff>